<commit_message>
feat: cleanup survey data a little
</commit_message>
<xml_diff>
--- a/data/pre/12-26 pre-survey data.xlsx
+++ b/data/pre/12-26 pre-survey data.xlsx
@@ -280,7 +280,7 @@
     <t xml:space="preserve">johnboscoaugustin@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Mavuko john bosco johnboscoaugustin@gmail.com</t>
+    <t xml:space="preserve">Mavuko john bosco</t>
   </si>
   <si>
     <t xml:space="preserve">Entre 4 mois et 1 an</t>
@@ -736,7 +736,7 @@
     <t xml:space="preserve">bahatikalangirosamuel@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bahati Samuel kalangiro </t>
+    <t xml:space="preserve">Bahati Samuel kalangiro </t>
   </si>
   <si>
     <t xml:space="preserve">Grammaire et orthographe </t>
@@ -5166,7 +5166,7 @@
     <t xml:space="preserve">davidjeanpierre772@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Jean-Pierre David / davidjeanpierre772@gmail.com</t>
+    <t xml:space="preserve">Jean-Pierre David</t>
   </si>
   <si>
     <t xml:space="preserve">6-12 ans</t>
@@ -5193,7 +5193,7 @@
     <t xml:space="preserve">prospereedno27@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Edno prospère Prospereedno27@gmail.com</t>
+    <t xml:space="preserve">Edno prospère</t>
   </si>
   <si>
     <t xml:space="preserve">13-18 ans</t>
@@ -5286,7 +5286,7 @@
     <t xml:space="preserve">altanasrodney@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Altanas Rodney altanasrodney@gmail.com </t>
+    <t xml:space="preserve">Altanas Rodney</t>
   </si>
   <si>
     <t xml:space="preserve">Ecouter</t>
@@ -5307,7 +5307,7 @@
     <t xml:space="preserve">9/23/2025 9:45:21</t>
   </si>
   <si>
-    <t xml:space="preserve">Kuzinda Amisi, jeannotamisi8@gmail.com</t>
+    <t xml:space="preserve">Kuzinda Amisi</t>
   </si>
   <si>
     <t xml:space="preserve">Lire et écrire </t>
@@ -6327,7 +6327,7 @@
     <t xml:space="preserve">rbalebanga@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve"> RamazaniBalebanga    rbalebanga@gmail.com</t>
+    <t xml:space="preserve">Ramazani Balebanga</t>
   </si>
   <si>
     <t xml:space="preserve">Les expressions anglaise et les proverbes</t>
@@ -6348,7 +6348,7 @@
     <t xml:space="preserve">9/28/2025 5:06:02</t>
   </si>
   <si>
-    <t xml:space="preserve">Balibuza jacques, yakobobalibuzajacques@gmail.com</t>
+    <t xml:space="preserve">Balibuza jacques</t>
   </si>
   <si>
     <t xml:space="preserve">Manque d'encandrement édifiant </t>
@@ -6567,7 +6567,7 @@
     <t xml:space="preserve">mbalapatrick054@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Patrick mbala mbalapatrick054@gmail.com</t>
+    <t xml:space="preserve">Patrick mbala</t>
   </si>
   <si>
     <t xml:space="preserve">Conversation et lire</t>
@@ -6588,7 +6588,7 @@
     <t xml:space="preserve">jacksonmapendo2022@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Nom: Mapendo Jackson. Adresse e-mail: jacksonmapendo2022@gmail.com</t>
+    <t xml:space="preserve">Mapendo Jackson</t>
   </si>
   <si>
     <t xml:space="preserve">Comprendre et parler rapidement dans les conversations quotidiennes.
@@ -9740,10 +9740,10 @@
   </sheetPr>
   <dimension ref="A1:BG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E409" activeCellId="0" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3515625" defaultRowHeight="20.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10123,7 +10123,7 @@
       <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -24188,10 +24188,10 @@
       <c r="C132" s="3" t="s">
         <v>1066</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="0"/>
+      <c r="E132" s="3" t="s">
         <v>1067</v>
       </c>
-      <c r="E132" s="8"/>
       <c r="F132" s="3" t="s">
         <v>1039</v>
       </c>
@@ -24319,10 +24319,10 @@
       <c r="C133" s="3" t="s">
         <v>1073</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D133" s="0"/>
+      <c r="E133" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="E133" s="8"/>
       <c r="F133" s="3" t="s">
         <v>1039</v>
       </c>
@@ -24450,10 +24450,10 @@
       <c r="C134" s="3" t="s">
         <v>1080</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="0"/>
+      <c r="E134" s="3" t="s">
         <v>1081</v>
       </c>
-      <c r="E134" s="8"/>
       <c r="F134" s="3" t="s">
         <v>73</v>
       </c>
@@ -24581,10 +24581,10 @@
       <c r="C135" s="3" t="s">
         <v>1087</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D135" s="0"/>
+      <c r="E135" s="3" t="s">
         <v>1088</v>
       </c>
-      <c r="E135" s="8"/>
       <c r="F135" s="3" t="s">
         <v>1039</v>
       </c>
@@ -24712,10 +24712,10 @@
       <c r="C136" s="3" t="s">
         <v>1093</v>
       </c>
-      <c r="D136" s="3" t="s">
+      <c r="D136" s="0"/>
+      <c r="E136" s="3" t="s">
         <v>1094</v>
       </c>
-      <c r="E136" s="8"/>
       <c r="F136" s="3" t="s">
         <v>1039</v>
       </c>
@@ -24843,10 +24843,10 @@
       <c r="C137" s="3" t="s">
         <v>1100</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D137" s="0"/>
+      <c r="E137" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="E137" s="8"/>
       <c r="F137" s="3" t="s">
         <v>1102</v>
       </c>
@@ -24974,10 +24974,10 @@
       <c r="C138" s="3" t="s">
         <v>1108</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D138" s="0"/>
+      <c r="E138" s="3" t="s">
         <v>1109</v>
       </c>
-      <c r="E138" s="8"/>
       <c r="F138" s="3" t="s">
         <v>73</v>
       </c>
@@ -25105,10 +25105,10 @@
       <c r="C139" s="3" t="s">
         <v>1115</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="0"/>
+      <c r="E139" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="E139" s="8"/>
       <c r="F139" s="3" t="s">
         <v>196</v>
       </c>
@@ -25236,10 +25236,10 @@
       <c r="C140" s="3" t="s">
         <v>1122</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D140" s="0"/>
+      <c r="E140" s="3" t="s">
         <v>1123</v>
       </c>
-      <c r="E140" s="8"/>
       <c r="F140" s="3" t="s">
         <v>73</v>
       </c>
@@ -25367,10 +25367,10 @@
       <c r="C141" s="3" t="s">
         <v>1130</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D141" s="0"/>
+      <c r="E141" s="3" t="s">
         <v>1131</v>
       </c>
-      <c r="E141" s="8"/>
       <c r="F141" s="3" t="s">
         <v>1039</v>
       </c>
@@ -25498,10 +25498,10 @@
       <c r="C142" s="3" t="s">
         <v>1137</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D142" s="0"/>
+      <c r="E142" s="3" t="s">
         <v>1138</v>
       </c>
-      <c r="E142" s="8"/>
       <c r="F142" s="3" t="s">
         <v>73</v>
       </c>
@@ -25629,10 +25629,10 @@
       <c r="C143" s="3" t="s">
         <v>1143</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D143" s="0"/>
+      <c r="E143" s="3" t="s">
         <v>1144</v>
       </c>
-      <c r="E143" s="8"/>
       <c r="F143" s="3" t="s">
         <v>73</v>
       </c>
@@ -25760,10 +25760,10 @@
       <c r="C144" s="3" t="s">
         <v>1147</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="0"/>
+      <c r="E144" s="3" t="s">
         <v>1148</v>
       </c>
-      <c r="E144" s="8"/>
       <c r="F144" s="3" t="s">
         <v>1102</v>
       </c>
@@ -25891,10 +25891,10 @@
       <c r="C145" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="D145" s="3" t="s">
+      <c r="D145" s="0"/>
+      <c r="E145" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="E145" s="8"/>
       <c r="F145" s="3" t="s">
         <v>73</v>
       </c>
@@ -26022,10 +26022,10 @@
       <c r="C146" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D146" s="0"/>
+      <c r="E146" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="E146" s="8"/>
       <c r="F146" s="3" t="s">
         <v>196</v>
       </c>
@@ -26153,10 +26153,10 @@
       <c r="C147" s="3" t="s">
         <v>1164</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="0"/>
+      <c r="E147" s="3" t="s">
         <v>1165</v>
       </c>
-      <c r="E147" s="8"/>
       <c r="F147" s="3" t="s">
         <v>1039</v>
       </c>
@@ -26284,10 +26284,10 @@
       <c r="C148" s="3" t="s">
         <v>1171</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="0"/>
+      <c r="E148" s="3" t="s">
         <v>1172</v>
       </c>
-      <c r="E148" s="8"/>
       <c r="F148" s="3" t="s">
         <v>73</v>
       </c>
@@ -26415,10 +26415,10 @@
       <c r="C149" s="3" t="s">
         <v>1177</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="0"/>
+      <c r="E149" s="3" t="s">
         <v>1178</v>
       </c>
-      <c r="E149" s="8"/>
       <c r="F149" s="3" t="s">
         <v>73</v>
       </c>
@@ -26546,10 +26546,10 @@
       <c r="C150" s="3" t="s">
         <v>1184</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D150" s="0"/>
+      <c r="E150" s="3" t="s">
         <v>1185</v>
       </c>
-      <c r="E150" s="8"/>
       <c r="F150" s="3" t="s">
         <v>73</v>
       </c>
@@ -26677,10 +26677,10 @@
       <c r="C151" s="3" t="s">
         <v>1190</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="0"/>
+      <c r="E151" s="3" t="s">
         <v>1191</v>
       </c>
-      <c r="E151" s="8"/>
       <c r="F151" s="3" t="s">
         <v>1039</v>
       </c>
@@ -26808,10 +26808,10 @@
       <c r="C152" s="3" t="s">
         <v>1195</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D152" s="0"/>
+      <c r="E152" s="3" t="s">
         <v>1196</v>
       </c>
-      <c r="E152" s="8"/>
       <c r="F152" s="3" t="s">
         <v>73</v>
       </c>
@@ -26939,10 +26939,10 @@
       <c r="C153" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D153" s="0"/>
+      <c r="E153" s="3" t="s">
         <v>1201</v>
       </c>
-      <c r="E153" s="8"/>
       <c r="F153" s="3" t="s">
         <v>196</v>
       </c>
@@ -27070,10 +27070,10 @@
       <c r="C154" s="3" t="s">
         <v>1206</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="0"/>
+      <c r="E154" s="3" t="s">
         <v>1207</v>
       </c>
-      <c r="E154" s="8"/>
       <c r="F154" s="3" t="s">
         <v>1039</v>
       </c>
@@ -27201,10 +27201,10 @@
       <c r="C155" s="3" t="s">
         <v>1212</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D155" s="0"/>
+      <c r="E155" s="3" t="s">
         <v>1213</v>
       </c>
-      <c r="E155" s="8"/>
       <c r="F155" s="3" t="s">
         <v>1039</v>
       </c>
@@ -27332,10 +27332,10 @@
       <c r="C156" s="3" t="s">
         <v>1219</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D156" s="0"/>
+      <c r="E156" s="3" t="s">
         <v>1220</v>
       </c>
-      <c r="E156" s="8"/>
       <c r="F156" s="3" t="s">
         <v>1039</v>
       </c>
@@ -27463,10 +27463,10 @@
       <c r="C157" s="3" t="s">
         <v>1226</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="0"/>
+      <c r="E157" s="3" t="s">
         <v>1227</v>
       </c>
-      <c r="E157" s="8"/>
       <c r="F157" s="3" t="s">
         <v>196</v>
       </c>
@@ -27594,10 +27594,10 @@
       <c r="C158" s="3" t="s">
         <v>1228</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D158" s="0"/>
+      <c r="E158" s="3" t="s">
         <v>1229</v>
       </c>
-      <c r="E158" s="8"/>
       <c r="F158" s="3" t="s">
         <v>196</v>
       </c>
@@ -27725,10 +27725,10 @@
       <c r="C159" s="3" t="s">
         <v>1231</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D159" s="0"/>
+      <c r="E159" s="3" t="s">
         <v>1232</v>
       </c>
-      <c r="E159" s="8"/>
       <c r="F159" s="3" t="s">
         <v>73</v>
       </c>
@@ -27856,10 +27856,10 @@
       <c r="C160" s="3" t="s">
         <v>1237</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D160" s="0"/>
+      <c r="E160" s="3" t="s">
         <v>1238</v>
       </c>
-      <c r="E160" s="8"/>
       <c r="F160" s="3" t="s">
         <v>196</v>
       </c>
@@ -27987,10 +27987,10 @@
       <c r="C161" s="3" t="s">
         <v>1242</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D161" s="0"/>
+      <c r="E161" s="3" t="s">
         <v>1243</v>
       </c>
-      <c r="E161" s="8"/>
       <c r="F161" s="3" t="s">
         <v>1039</v>
       </c>
@@ -28118,10 +28118,10 @@
       <c r="C162" s="3" t="s">
         <v>1249</v>
       </c>
-      <c r="D162" s="3" t="s">
+      <c r="D162" s="0"/>
+      <c r="E162" s="3" t="s">
         <v>1250</v>
       </c>
-      <c r="E162" s="8"/>
       <c r="F162" s="3" t="s">
         <v>196</v>
       </c>
@@ -28249,10 +28249,10 @@
       <c r="C163" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="D163" s="3" t="s">
+      <c r="D163" s="0"/>
+      <c r="E163" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="E163" s="8"/>
       <c r="F163" s="3" t="s">
         <v>73</v>
       </c>
@@ -28380,10 +28380,10 @@
       <c r="C164" s="3" t="s">
         <v>1261</v>
       </c>
-      <c r="D164" s="3" t="s">
+      <c r="D164" s="0"/>
+      <c r="E164" s="3" t="s">
         <v>1262</v>
       </c>
-      <c r="E164" s="8"/>
       <c r="F164" s="3" t="s">
         <v>1039</v>
       </c>
@@ -28511,10 +28511,10 @@
       <c r="C165" s="3" t="s">
         <v>1268</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="D165" s="0"/>
+      <c r="E165" s="3" t="s">
         <v>1269</v>
       </c>
-      <c r="E165" s="8"/>
       <c r="F165" s="3" t="s">
         <v>196</v>
       </c>
@@ -28642,10 +28642,10 @@
       <c r="C166" s="3" t="s">
         <v>1275</v>
       </c>
-      <c r="D166" s="3" t="s">
+      <c r="D166" s="0"/>
+      <c r="E166" s="3" t="s">
         <v>1276</v>
       </c>
-      <c r="E166" s="8"/>
       <c r="F166" s="3" t="s">
         <v>73</v>
       </c>
@@ -28773,10 +28773,10 @@
       <c r="C167" s="3" t="s">
         <v>1282</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D167" s="0"/>
+      <c r="E167" s="3" t="s">
         <v>1283</v>
       </c>
-      <c r="E167" s="8"/>
       <c r="F167" s="3" t="s">
         <v>73</v>
       </c>
@@ -28904,10 +28904,10 @@
       <c r="C168" s="3" t="s">
         <v>1289</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D168" s="0"/>
+      <c r="E168" s="3" t="s">
         <v>1290</v>
       </c>
-      <c r="E168" s="8"/>
       <c r="F168" s="3" t="s">
         <v>73</v>
       </c>
@@ -29035,10 +29035,10 @@
       <c r="C169" s="3" t="s">
         <v>1296</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D169" s="0"/>
+      <c r="E169" s="3" t="s">
         <v>1297</v>
       </c>
-      <c r="E169" s="8"/>
       <c r="F169" s="3" t="s">
         <v>1039</v>
       </c>
@@ -29166,10 +29166,10 @@
       <c r="C170" s="3" t="s">
         <v>1303</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D170" s="0"/>
+      <c r="E170" s="3" t="s">
         <v>1304</v>
       </c>
-      <c r="E170" s="8"/>
       <c r="F170" s="3" t="s">
         <v>196</v>
       </c>
@@ -29297,10 +29297,10 @@
       <c r="C171" s="3" t="s">
         <v>1309</v>
       </c>
-      <c r="D171" s="3" t="s">
+      <c r="D171" s="0"/>
+      <c r="E171" s="3" t="s">
         <v>1310</v>
       </c>
-      <c r="E171" s="8"/>
       <c r="F171" s="3" t="s">
         <v>73</v>
       </c>
@@ -29428,10 +29428,10 @@
       <c r="C172" s="3" t="s">
         <v>1316</v>
       </c>
-      <c r="D172" s="3" t="s">
+      <c r="D172" s="0"/>
+      <c r="E172" s="3" t="s">
         <v>1317</v>
       </c>
-      <c r="E172" s="8"/>
       <c r="F172" s="3" t="s">
         <v>1039</v>
       </c>
@@ -29559,10 +29559,10 @@
       <c r="C173" s="3" t="s">
         <v>1323</v>
       </c>
-      <c r="D173" s="3" t="s">
+      <c r="D173" s="0"/>
+      <c r="E173" s="3" t="s">
         <v>1324</v>
       </c>
-      <c r="E173" s="8"/>
       <c r="F173" s="3" t="s">
         <v>1039</v>
       </c>
@@ -29690,10 +29690,10 @@
       <c r="C174" s="3" t="s">
         <v>1330</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D174" s="0"/>
+      <c r="E174" s="3" t="s">
         <v>1331</v>
       </c>
-      <c r="E174" s="8"/>
       <c r="F174" s="3" t="s">
         <v>196</v>
       </c>
@@ -29821,10 +29821,10 @@
       <c r="C175" s="3" t="s">
         <v>1336</v>
       </c>
-      <c r="D175" s="3" t="s">
+      <c r="D175" s="0"/>
+      <c r="E175" s="3" t="s">
         <v>1337</v>
       </c>
-      <c r="E175" s="8"/>
       <c r="F175" s="3" t="s">
         <v>1039</v>
       </c>
@@ -29952,10 +29952,10 @@
       <c r="C176" s="3" t="s">
         <v>1339</v>
       </c>
-      <c r="D176" s="3" t="s">
+      <c r="D176" s="0"/>
+      <c r="E176" s="3" t="s">
         <v>1340</v>
       </c>
-      <c r="E176" s="8"/>
       <c r="F176" s="3" t="s">
         <v>73</v>
       </c>
@@ -30083,10 +30083,10 @@
       <c r="C177" s="3" t="s">
         <v>1346</v>
       </c>
-      <c r="D177" s="3" t="s">
+      <c r="D177" s="0"/>
+      <c r="E177" s="3" t="s">
         <v>1347</v>
       </c>
-      <c r="E177" s="8"/>
       <c r="F177" s="3" t="s">
         <v>73</v>
       </c>
@@ -30214,10 +30214,10 @@
       <c r="C178" s="3" t="s">
         <v>1353</v>
       </c>
-      <c r="D178" s="3" t="s">
+      <c r="D178" s="0"/>
+      <c r="E178" s="3" t="s">
         <v>1354</v>
       </c>
-      <c r="E178" s="8"/>
       <c r="F178" s="3" t="s">
         <v>73</v>
       </c>
@@ -30345,10 +30345,10 @@
       <c r="C179" s="3" t="s">
         <v>1359</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="D179" s="0"/>
+      <c r="E179" s="3" t="s">
         <v>1360</v>
       </c>
-      <c r="E179" s="8"/>
       <c r="F179" s="3" t="s">
         <v>73</v>
       </c>
@@ -30476,10 +30476,10 @@
       <c r="C180" s="3" t="s">
         <v>1366</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D180" s="0"/>
+      <c r="E180" s="3" t="s">
         <v>1367</v>
       </c>
-      <c r="E180" s="8"/>
       <c r="F180" s="3" t="s">
         <v>73</v>
       </c>
@@ -30607,10 +30607,10 @@
       <c r="C181" s="3" t="s">
         <v>1373</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="D181" s="0"/>
+      <c r="E181" s="3" t="s">
         <v>1374</v>
       </c>
-      <c r="E181" s="8"/>
       <c r="F181" s="3" t="s">
         <v>1102</v>
       </c>
@@ -30738,10 +30738,10 @@
       <c r="C182" s="3" t="s">
         <v>1380</v>
       </c>
-      <c r="D182" s="3" t="s">
+      <c r="D182" s="0"/>
+      <c r="E182" s="3" t="s">
         <v>1381</v>
       </c>
-      <c r="E182" s="8"/>
       <c r="F182" s="3" t="s">
         <v>1102</v>
       </c>
@@ -30869,10 +30869,10 @@
       <c r="C183" s="3" t="s">
         <v>1387</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D183" s="0"/>
+      <c r="E183" s="3" t="s">
         <v>1388</v>
       </c>
-      <c r="E183" s="8"/>
       <c r="F183" s="3" t="s">
         <v>1102</v>
       </c>
@@ -31000,10 +31000,10 @@
       <c r="C184" s="3" t="s">
         <v>1394</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="D184" s="0"/>
+      <c r="E184" s="3" t="s">
         <v>1395</v>
       </c>
-      <c r="E184" s="8"/>
       <c r="F184" s="3" t="s">
         <v>196</v>
       </c>
@@ -31131,10 +31131,10 @@
       <c r="C185" s="3" t="s">
         <v>1401</v>
       </c>
-      <c r="D185" s="3" t="s">
+      <c r="D185" s="0"/>
+      <c r="E185" s="3" t="s">
         <v>1402</v>
       </c>
-      <c r="E185" s="8"/>
       <c r="F185" s="3" t="s">
         <v>196</v>
       </c>
@@ -31262,10 +31262,10 @@
       <c r="C186" s="3" t="s">
         <v>1408</v>
       </c>
-      <c r="D186" s="3" t="s">
+      <c r="D186" s="0"/>
+      <c r="E186" s="3" t="s">
         <v>1409</v>
       </c>
-      <c r="E186" s="8"/>
       <c r="F186" s="3" t="s">
         <v>73</v>
       </c>
@@ -31393,10 +31393,10 @@
       <c r="C187" s="3" t="s">
         <v>1414</v>
       </c>
-      <c r="D187" s="3" t="s">
+      <c r="D187" s="0"/>
+      <c r="E187" s="3" t="s">
         <v>1415</v>
       </c>
-      <c r="E187" s="8"/>
       <c r="F187" s="3" t="s">
         <v>1039</v>
       </c>
@@ -31524,10 +31524,10 @@
       <c r="C188" s="3" t="s">
         <v>1420</v>
       </c>
-      <c r="D188" s="3" t="s">
+      <c r="D188" s="0"/>
+      <c r="E188" s="3" t="s">
         <v>1421</v>
       </c>
-      <c r="E188" s="8"/>
       <c r="F188" s="3" t="s">
         <v>73</v>
       </c>
@@ -31655,10 +31655,10 @@
       <c r="C189" s="3" t="s">
         <v>1425</v>
       </c>
-      <c r="D189" s="3" t="s">
+      <c r="D189" s="0"/>
+      <c r="E189" s="3" t="s">
         <v>1426</v>
       </c>
-      <c r="E189" s="8"/>
       <c r="F189" s="3" t="s">
         <v>73</v>
       </c>
@@ -31786,10 +31786,10 @@
       <c r="C190" s="3" t="s">
         <v>1432</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D190" s="0"/>
+      <c r="E190" s="3" t="s">
         <v>1433</v>
       </c>
-      <c r="E190" s="8"/>
       <c r="F190" s="3" t="s">
         <v>196</v>
       </c>
@@ -31917,10 +31917,10 @@
       <c r="C191" s="3" t="s">
         <v>1439</v>
       </c>
-      <c r="D191" s="3" t="s">
+      <c r="D191" s="0"/>
+      <c r="E191" s="3" t="s">
         <v>1440</v>
       </c>
-      <c r="E191" s="8"/>
       <c r="F191" s="3" t="s">
         <v>73</v>
       </c>
@@ -32048,10 +32048,10 @@
       <c r="C192" s="3" t="s">
         <v>1446</v>
       </c>
-      <c r="D192" s="3" t="s">
+      <c r="D192" s="0"/>
+      <c r="E192" s="3" t="s">
         <v>1447</v>
       </c>
-      <c r="E192" s="8"/>
       <c r="F192" s="3" t="s">
         <v>196</v>
       </c>
@@ -32179,10 +32179,10 @@
       <c r="C193" s="3" t="s">
         <v>1453</v>
       </c>
-      <c r="D193" s="3" t="s">
+      <c r="D193" s="0"/>
+      <c r="E193" s="3" t="s">
         <v>1454</v>
       </c>
-      <c r="E193" s="8"/>
       <c r="F193" s="3" t="s">
         <v>73</v>
       </c>
@@ -32310,10 +32310,10 @@
       <c r="C194" s="3" t="s">
         <v>1460</v>
       </c>
-      <c r="D194" s="3" t="s">
+      <c r="D194" s="0"/>
+      <c r="E194" s="3" t="s">
         <v>1461</v>
       </c>
-      <c r="E194" s="8"/>
       <c r="F194" s="3" t="s">
         <v>73</v>
       </c>
@@ -32441,10 +32441,10 @@
       <c r="C195" s="3" t="s">
         <v>1467</v>
       </c>
-      <c r="D195" s="3" t="s">
+      <c r="D195" s="0"/>
+      <c r="E195" s="3" t="s">
         <v>1468</v>
       </c>
-      <c r="E195" s="8"/>
       <c r="F195" s="3" t="s">
         <v>73</v>
       </c>
@@ -32572,10 +32572,10 @@
       <c r="C196" s="3" t="s">
         <v>1474</v>
       </c>
-      <c r="D196" s="3" t="s">
+      <c r="D196" s="0"/>
+      <c r="E196" s="3" t="s">
         <v>1475</v>
       </c>
-      <c r="E196" s="8"/>
       <c r="F196" s="3" t="s">
         <v>73</v>
       </c>
@@ -32703,10 +32703,10 @@
       <c r="C197" s="3" t="s">
         <v>1481</v>
       </c>
-      <c r="D197" s="3" t="s">
+      <c r="D197" s="0"/>
+      <c r="E197" s="3" t="s">
         <v>1482</v>
       </c>
-      <c r="E197" s="8"/>
       <c r="F197" s="3" t="s">
         <v>1102</v>
       </c>
@@ -32834,10 +32834,10 @@
       <c r="C198" s="3" t="s">
         <v>1488</v>
       </c>
-      <c r="D198" s="3" t="s">
+      <c r="D198" s="0"/>
+      <c r="E198" s="3" t="s">
         <v>1489</v>
       </c>
-      <c r="E198" s="8"/>
       <c r="F198" s="3" t="s">
         <v>73</v>
       </c>
@@ -32965,10 +32965,10 @@
       <c r="C199" s="3" t="s">
         <v>1495</v>
       </c>
-      <c r="D199" s="3" t="s">
+      <c r="D199" s="0"/>
+      <c r="E199" s="3" t="s">
         <v>1496</v>
       </c>
-      <c r="E199" s="8"/>
       <c r="F199" s="3" t="s">
         <v>1102</v>
       </c>
@@ -33096,10 +33096,10 @@
       <c r="C200" s="3" t="s">
         <v>1502</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D200" s="0"/>
+      <c r="E200" s="3" t="s">
         <v>1503</v>
       </c>
-      <c r="E200" s="8"/>
       <c r="F200" s="3" t="s">
         <v>1102</v>
       </c>
@@ -33227,10 +33227,10 @@
       <c r="C201" s="3" t="s">
         <v>1509</v>
       </c>
-      <c r="D201" s="3" t="s">
+      <c r="D201" s="0"/>
+      <c r="E201" s="3" t="s">
         <v>1510</v>
       </c>
-      <c r="E201" s="8"/>
       <c r="F201" s="3" t="s">
         <v>1102</v>
       </c>
@@ -33358,10 +33358,10 @@
       <c r="C202" s="3" t="s">
         <v>1516</v>
       </c>
-      <c r="D202" s="3" t="s">
+      <c r="D202" s="0"/>
+      <c r="E202" s="3" t="s">
         <v>1517</v>
       </c>
-      <c r="E202" s="8"/>
       <c r="F202" s="3" t="s">
         <v>196</v>
       </c>
@@ -33489,10 +33489,10 @@
       <c r="C203" s="3" t="s">
         <v>1522</v>
       </c>
-      <c r="D203" s="3" t="s">
+      <c r="D203" s="0"/>
+      <c r="E203" s="3" t="s">
         <v>1523</v>
       </c>
-      <c r="E203" s="8"/>
       <c r="F203" s="3" t="s">
         <v>196</v>
       </c>
@@ -33620,10 +33620,10 @@
       <c r="C204" s="3" t="s">
         <v>1529</v>
       </c>
-      <c r="D204" s="3" t="s">
+      <c r="D204" s="0"/>
+      <c r="E204" s="3" t="s">
         <v>1530</v>
       </c>
-      <c r="E204" s="8"/>
       <c r="F204" s="3" t="s">
         <v>73</v>
       </c>
@@ -33751,10 +33751,10 @@
       <c r="C205" s="3" t="s">
         <v>1536</v>
       </c>
-      <c r="D205" s="3" t="s">
+      <c r="D205" s="0"/>
+      <c r="E205" s="3" t="s">
         <v>1537</v>
       </c>
-      <c r="E205" s="8"/>
       <c r="F205" s="3" t="s">
         <v>196</v>
       </c>
@@ -33882,10 +33882,10 @@
       <c r="C206" s="3" t="s">
         <v>1543</v>
       </c>
-      <c r="D206" s="3" t="s">
+      <c r="D206" s="0"/>
+      <c r="E206" s="3" t="s">
         <v>1544</v>
       </c>
-      <c r="E206" s="8"/>
       <c r="F206" s="3" t="s">
         <v>73</v>
       </c>
@@ -34013,10 +34013,10 @@
       <c r="C207" s="3" t="s">
         <v>1550</v>
       </c>
-      <c r="D207" s="3" t="s">
+      <c r="D207" s="0"/>
+      <c r="E207" s="3" t="s">
         <v>1551</v>
       </c>
-      <c r="E207" s="8"/>
       <c r="F207" s="3" t="s">
         <v>196</v>
       </c>
@@ -34144,10 +34144,10 @@
       <c r="C208" s="3" t="s">
         <v>1555</v>
       </c>
-      <c r="D208" s="3" t="s">
+      <c r="D208" s="0"/>
+      <c r="E208" s="3" t="s">
         <v>1556</v>
       </c>
-      <c r="E208" s="8"/>
       <c r="F208" s="3" t="s">
         <v>196</v>
       </c>
@@ -34275,10 +34275,10 @@
       <c r="C209" s="3" t="s">
         <v>1562</v>
       </c>
-      <c r="D209" s="3" t="s">
+      <c r="D209" s="0"/>
+      <c r="E209" s="3" t="s">
         <v>1563</v>
       </c>
-      <c r="E209" s="8"/>
       <c r="F209" s="3" t="s">
         <v>196</v>
       </c>
@@ -34406,10 +34406,10 @@
       <c r="C210" s="3" t="s">
         <v>1569</v>
       </c>
-      <c r="D210" s="3" t="s">
+      <c r="D210" s="0"/>
+      <c r="E210" s="3" t="s">
         <v>1570</v>
       </c>
-      <c r="E210" s="8"/>
       <c r="F210" s="3" t="s">
         <v>196</v>
       </c>
@@ -34537,10 +34537,10 @@
       <c r="C211" s="3" t="s">
         <v>1574</v>
       </c>
-      <c r="D211" s="3" t="s">
+      <c r="D211" s="0"/>
+      <c r="E211" s="3" t="s">
         <v>1575</v>
       </c>
-      <c r="E211" s="8"/>
       <c r="F211" s="3" t="s">
         <v>196</v>
       </c>
@@ -34668,10 +34668,10 @@
       <c r="C212" s="3" t="s">
         <v>1579</v>
       </c>
-      <c r="D212" s="3" t="s">
+      <c r="D212" s="0"/>
+      <c r="E212" s="3" t="s">
         <v>1580</v>
       </c>
-      <c r="E212" s="8"/>
       <c r="F212" s="3" t="s">
         <v>1102</v>
       </c>
@@ -34799,10 +34799,10 @@
       <c r="C213" s="3" t="s">
         <v>1586</v>
       </c>
-      <c r="D213" s="3" t="s">
+      <c r="D213" s="0"/>
+      <c r="E213" s="3" t="s">
         <v>1587</v>
       </c>
-      <c r="E213" s="8"/>
       <c r="F213" s="3" t="s">
         <v>1102</v>
       </c>
@@ -34930,10 +34930,10 @@
       <c r="C214" s="3" t="s">
         <v>1593</v>
       </c>
-      <c r="D214" s="3" t="s">
+      <c r="D214" s="0"/>
+      <c r="E214" s="3" t="s">
         <v>1594</v>
       </c>
-      <c r="E214" s="8"/>
       <c r="F214" s="3" t="s">
         <v>1102</v>
       </c>
@@ -35061,10 +35061,10 @@
       <c r="C215" s="3" t="s">
         <v>1600</v>
       </c>
-      <c r="D215" s="3" t="s">
+      <c r="D215" s="0"/>
+      <c r="E215" s="3" t="s">
         <v>1601</v>
       </c>
-      <c r="E215" s="8"/>
       <c r="F215" s="3" t="s">
         <v>1102</v>
       </c>
@@ -35192,10 +35192,10 @@
       <c r="C216" s="3" t="s">
         <v>1607</v>
       </c>
-      <c r="D216" s="3" t="s">
+      <c r="D216" s="0"/>
+      <c r="E216" s="3" t="s">
         <v>1608</v>
       </c>
-      <c r="E216" s="8"/>
       <c r="F216" s="3" t="s">
         <v>73</v>
       </c>
@@ -35323,10 +35323,10 @@
       <c r="C217" s="3" t="s">
         <v>1614</v>
       </c>
-      <c r="D217" s="3" t="s">
+      <c r="D217" s="0"/>
+      <c r="E217" s="3" t="s">
         <v>1615</v>
       </c>
-      <c r="E217" s="8"/>
       <c r="F217" s="3" t="s">
         <v>1102</v>
       </c>
@@ -35625,7 +35625,7 @@
       <c r="D220" s="4" t="s">
         <v>1644</v>
       </c>
-      <c r="E220" s="4" t="s">
+      <c r="E220" s="0" t="s">
         <v>1645</v>
       </c>
       <c r="F220" s="7"/>
@@ -35709,7 +35709,7 @@
       <c r="D221" s="4" t="s">
         <v>1653</v>
       </c>
-      <c r="E221" s="4" t="s">
+      <c r="E221" s="0" t="s">
         <v>1654</v>
       </c>
       <c r="F221" s="7"/>
@@ -36127,7 +36127,7 @@
       <c r="D226" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E226" s="4" t="s">
+      <c r="E226" s="0" t="s">
         <v>1692</v>
       </c>
       <c r="F226" s="3" t="s">
@@ -41407,7 +41407,7 @@
       <c r="D274" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E274" s="4" t="s">
+      <c r="E274" s="0" t="s">
         <v>2038</v>
       </c>
       <c r="F274" s="3" t="s">
@@ -42617,7 +42617,7 @@
       <c r="D285" s="4" t="s">
         <v>2117</v>
       </c>
-      <c r="E285" s="4" t="s">
+      <c r="E285" s="0" t="s">
         <v>2118</v>
       </c>
       <c r="F285" s="3" t="s">
@@ -56799,343 +56799,334 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="jeannotamisi8@gmail.com"/>
     <hyperlink ref="D4" r:id="rId2" display="johnboscoaugustin@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId3" display="Mavuko john bosco johnboscoaugustin@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="yakobobalibuzajacques@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="kitumainimakeledeodate@gmail.com"/>
-    <hyperlink ref="D7" r:id="rId6" display="nondamulenga@gamil.com"/>
-    <hyperlink ref="D8" r:id="rId7" display="shimazephy6@gmail.com"/>
-    <hyperlink ref="D9" r:id="rId8" display="Agroanzuruni@gmail.com"/>
-    <hyperlink ref="D10" r:id="rId9" display="iragijeff@gmail.com"/>
-    <hyperlink ref="D11" r:id="rId10" display="kwizerajeanmarie53@gmail.com"/>
-    <hyperlink ref="D12" r:id="rId11" display="triomphebirenganya@gmail.om"/>
-    <hyperlink ref="D13" r:id="rId12" display="ausengimanaodette34@gmail.com"/>
-    <hyperlink ref="AI13" r:id="rId13" display="Le plus difficile, c’est de ne pas pouvoir transmettre l’émotion ou l’intention exacte ça peut créer des malentendus ou briser la connexion.si le sujet est Mal étendu &#10;"/>
-    <hyperlink ref="D14" r:id="rId14" display="cimushoshere@gmail.com"/>
-    <hyperlink ref="D15" r:id="rId15" display="eddymulindwa013@gmail.com"/>
-    <hyperlink ref="D16" r:id="rId16" display="bizimanajuvenal@gmail.com"/>
-    <hyperlink ref="D17" r:id="rId17" display="conforgeca@gmail.com"/>
-    <hyperlink ref="D18" r:id="rId18" display="jacquesbahati37@gmail.com"/>
-    <hyperlink ref="D19" r:id="rId19" display="denismunguiko12@gmail.com"/>
-    <hyperlink ref="D20" r:id="rId20" display="hopevisioneenterprise@gmail.com"/>
-    <hyperlink ref="D21" r:id="rId21" display="bahatikalangirosamuel@gmail.com"/>
-    <hyperlink ref="D22" r:id="rId22" display="benjaminngota@gmail.com"/>
-    <hyperlink ref="D23" r:id="rId23" display="kipondaruvukisha@gmail.com"/>
-    <hyperlink ref="D24" r:id="rId24" display="mauwaizakiena@gmail.com"/>
-    <hyperlink ref="D25" r:id="rId25" display="irandukundafleury@gmail.com"/>
-    <hyperlink ref="D26" r:id="rId26" display="uwizeyimanapaskarine@gmail.com"/>
-    <hyperlink ref="D27" r:id="rId27" display="mugishablaise961@gmail.com"/>
-    <hyperlink ref="D28" r:id="rId28" display="herietteliwilana@gmail.com"/>
-    <hyperlink ref="D29" r:id="rId29" display="vanessashimirimana@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId30" display="imaniyaleoboutros2@gmail.com"/>
-    <hyperlink ref="D31" r:id="rId31" display="winvestine@gmail.com"/>
-    <hyperlink ref="D32" r:id="rId32" display="katingwamasanzeleo@gmail.com"/>
-    <hyperlink ref="D33" r:id="rId33" display="Innocentuwezosebareka@gamil.com"/>
-    <hyperlink ref="D34" r:id="rId34" display="Barakasebaraka@gmail.com"/>
-    <hyperlink ref="D35" r:id="rId35" display="kingjacksonmuleka@gmail.com"/>
-    <hyperlink ref="D36" r:id="rId36" display="johnmunguiko643@gmqil.com"/>
-    <hyperlink ref="D37" r:id="rId37" display="Naimasumami@gmail.com"/>
-    <hyperlink ref="D38" r:id="rId38" display="shabanikaffifa@gmail.com"/>
-    <hyperlink ref="D39" r:id="rId39" display="Akimanakelly@gmail.com"/>
-    <hyperlink ref="D40" r:id="rId40" display="Nyandubonybonny@gmail.com"/>
-    <hyperlink ref="D41" r:id="rId41" display="achizajeff@gmail.com"/>
-    <hyperlink ref="D42" r:id="rId42" display="clovisrashidi457@gmail.com"/>
-    <hyperlink ref="D43" r:id="rId43" display="somodtwagira@gmail.com"/>
-    <hyperlink ref="D44" r:id="rId44" display="Nadegendwangayesu@gmail.com"/>
-    <hyperlink ref="D45" r:id="rId45" display="gowingongwe@gmail.com"/>
-    <hyperlink ref="D46" r:id="rId46" display="misumbamitunga@gmail.com"/>
-    <hyperlink ref="D47" r:id="rId47" display="marcelinemungama@gmail.com"/>
-    <hyperlink ref="D48" r:id="rId48" display="Luson6@gmil.com"/>
-    <hyperlink ref="D49" r:id="rId49" display="mwaminichristel@gmail.com"/>
-    <hyperlink ref="D50" r:id="rId50" display="fistonbikuku@gmail.com"/>
-    <hyperlink ref="D51" r:id="rId51" display="mugishablaise961@gmail.com"/>
-    <hyperlink ref="D52" r:id="rId52" display="niwamungubalazi@gmail.com"/>
-    <hyperlink ref="D53" r:id="rId53" display="fifiviane@gmail.com"/>
-    <hyperlink ref="D54" r:id="rId54" display="joycemanirakiza6@gmail.com"/>
-    <hyperlink ref="D55" r:id="rId55" display="abwemkyombwechristophe@gmail.com"/>
-    <hyperlink ref="D56" r:id="rId56" display="shanikehonda6@gmail.com"/>
-    <hyperlink ref="D57" r:id="rId57" display="irakundeliesse@gmail.com"/>
-    <hyperlink ref="D58" r:id="rId58" display="hayarimanaclairia@gmail.com"/>
-    <hyperlink ref="D59" r:id="rId59" display="habiyambeemmanuel@gail.com"/>
-    <hyperlink ref="D60" r:id="rId60" display="espoirkalamo@gmail.com"/>
-    <hyperlink ref="D61" r:id="rId61" display="somodtwagira@gmail.com"/>
-    <hyperlink ref="D62" r:id="rId62" display="ernestmikato@gmail.com"/>
-    <hyperlink ref="D63" r:id="rId63" display="abrahamod@gmail.com"/>
-    <hyperlink ref="D64" r:id="rId64" display="kipondaruvukisha@gmail.com"/>
-    <hyperlink ref="D65" r:id="rId65" display="muzaliwarashidi93@gmail.com"/>
-    <hyperlink ref="D66" r:id="rId66" display="azizamwabwa@gmail.com"/>
-    <hyperlink ref="D67" r:id="rId67" display="fikiriwafikiri@gmail.com"/>
-    <hyperlink ref="D68" r:id="rId68" display="albertalka@gmail.com"/>
-    <hyperlink ref="D69" r:id="rId69" display="apolinaanna@gmail.com"/>
-    <hyperlink ref="D70" r:id="rId70" display="bisimwaciza387@gmail.com"/>
-    <hyperlink ref="D71" r:id="rId71" display="blaisebitangimana18@gmail.com"/>
-    <hyperlink ref="D72" r:id="rId72" display="bonynyandu@gmail.com"/>
-    <hyperlink ref="D73" r:id="rId73" display="cadeaungakani@gmail.com"/>
-    <hyperlink ref="D74" r:id="rId74" display="christellemwamini026@gmail.com"/>
-    <hyperlink ref="D75" r:id="rId75" display="cizaladent@gmail.com"/>
-    <hyperlink ref="D76" r:id="rId76" display="davidblessingjanvier@gmail.com"/>
-    <hyperlink ref="D77" r:id="rId77" display="delphinwingimana8@gmail.com"/>
-    <hyperlink ref="D78" r:id="rId78" display="dusabejisele@gmail.com"/>
-    <hyperlink ref="D79" r:id="rId79" display="dusengimanaodette34@gmail.com"/>
-    <hyperlink ref="D80" r:id="rId80" display="faidabimule@gmail.com"/>
-    <hyperlink ref="D81" r:id="rId81" display="fifiviane@gmail.com"/>
-    <hyperlink ref="D82" r:id="rId82" display="fikiriwafikiri@gmail.com"/>
-    <hyperlink ref="D83" r:id="rId83" display="gilbermukacho@gmail.com"/>
-    <hyperlink ref="D84" r:id="rId84" display="hayarimanaclairia@gmail.com"/>
-    <hyperlink ref="D85" r:id="rId85" display="ibrahimramazani@gmail.com"/>
-    <hyperlink ref="D86" r:id="rId86" display="kalamuespoire35@gmail.com"/>
-    <hyperlink ref="D87" r:id="rId87" display="kennygakwanya7@gmail.com"/>
-    <hyperlink ref="D88" r:id="rId88" display="kingnikolasngakani@gmail.com"/>
-    <hyperlink ref="D89" r:id="rId89" display="kwizerajeanmarie53@gmail.com"/>
-    <hyperlink ref="D90" r:id="rId90" display="mavukojohnbosco@gmail.com"/>
-    <hyperlink ref="D91" r:id="rId91" display="mosesnandogera@gmail.com"/>
-    <hyperlink ref="D92" r:id="rId92" display="mubaamos5@gmail.com"/>
-    <hyperlink ref="D93" r:id="rId93" display="mugishaabdulakarim48@gmail.com"/>
-    <hyperlink ref="D94" r:id="rId94" display="nduwimanadesire449@gmail.com"/>
-    <hyperlink ref="E94" r:id="rId95" display="nduwimanadesire449@gmail.com"/>
-    <hyperlink ref="D95" r:id="rId96" display="nishimwehassan@gmail.com"/>
-    <hyperlink ref="D96" r:id="rId97" display="ebuelayamungu@gmail.com"/>
-    <hyperlink ref="D97" r:id="rId98" display="josephjilardo@gmail.com"/>
-    <hyperlink ref="D98" r:id="rId99" display="januarybessinesjile@gmail.com"/>
-    <hyperlink ref="D99" r:id="rId100" display="farijikalukuli@gmail.com"/>
-    <hyperlink ref="D100" r:id="rId101" display="fidelematete@gmail.com"/>
-    <hyperlink ref="D101" r:id="rId102" display="kivulibko7@gmail.com"/>
-    <hyperlink ref="D102" r:id="rId103" display="juniormekhan60@gmail.com"/>
-    <hyperlink ref="D103" r:id="rId104" display="oscarmusabimana4@gmail.co"/>
-    <hyperlink ref="D104" r:id="rId105" display="mavulano5@gmail.com"/>
-    <hyperlink ref="D105" r:id="rId106" display="apendkieresi@gmail.com"/>
-    <hyperlink ref="D106" r:id="rId107" display="angelolokorai@gmail.com"/>
-    <hyperlink ref="D107" r:id="rId108" display="kwalibbko7@gmail.com"/>
-    <hyperlink ref="D108" r:id="rId109" display="mulenganonda1@gmail.com"/>
-    <hyperlink ref="D109" r:id="rId110" display="mugishaabdulakarim487@gmail.com"/>
-    <hyperlink ref="D110" r:id="rId111" display="tomthree190@gmail.com"/>
-    <hyperlink ref="D111" r:id="rId112" display="vincentnduwamungu48@gmail.com"/>
-    <hyperlink ref="D112" r:id="rId113" display="pacificnundu@gmail.com"/>
-    <hyperlink ref="D113" r:id="rId114" display="zainaswedi9@gmail.com"/>
-    <hyperlink ref="D114" r:id="rId115" display="wasalumiwasalumu@gmail.com"/>
-    <hyperlink ref="D115" r:id="rId116" display="olivier4@gmail.com"/>
-    <hyperlink ref="D116" r:id="rId117" display="achizajeff@gmail.com"/>
-    <hyperlink ref="D117" r:id="rId118" display="juniormekhan60@gmail.com"/>
-    <hyperlink ref="D118" r:id="rId119" display="alka01139@gmail.com"/>
-    <hyperlink ref="D119" r:id="rId120" display="f81925614@gmail.com"/>
-    <hyperlink ref="D120" r:id="rId121" display="apendkieresi@gmail.com"/>
-    <hyperlink ref="D121" r:id="rId122" display="chizabisimwa5@gmail.com"/>
-    <hyperlink ref="D122" r:id="rId123" display="angelolokorai@gmail.com"/>
-    <hyperlink ref="D123" r:id="rId124" display="imaniyaleoboutros2@gmail.com"/>
-    <hyperlink ref="D124" r:id="rId125" display="kivulibk07@gmail.com"/>
-    <hyperlink ref="D125" r:id="rId126" display="cholvalentines737@gmail.com"/>
-    <hyperlink ref="D126" r:id="rId127" display="meshefaustin@gmail.com"/>
-    <hyperlink ref="D127" r:id="rId128" display="mwaminichimanuka@gmail.com"/>
-    <hyperlink ref="D128" r:id="rId129" display="kwalibbko7@gmail.com"/>
-    <hyperlink ref="D129" r:id="rId130" display="kichonavenuelle@gmail.com"/>
-    <hyperlink ref="D130" r:id="rId131" display="stephenokech@gmail.com"/>
-    <hyperlink ref="D131" r:id="rId132" display="bizimanajuvenel120@gmail.com"/>
-    <hyperlink ref="D218" r:id="rId133" display="desirjeanedens75@gmail.com"/>
-    <hyperlink ref="D219" r:id="rId134" display="sandra.jean2@icloud.com"/>
-    <hyperlink ref="D220" r:id="rId135" display="davidjeanpierre772@gmail.com"/>
-    <hyperlink ref="E220" r:id="rId136" display="Jean-Pierre David / davidjeanpierre772@gmail.com"/>
-    <hyperlink ref="D221" r:id="rId137" display="prospereedno27@gmail.com"/>
-    <hyperlink ref="E221" r:id="rId138" display="Edno prospère Prospereedno27@gmail.com"/>
-    <hyperlink ref="D222" r:id="rId139" display="charleswilkendy80@gmail.com"/>
-    <hyperlink ref="E222" r:id="rId140" display="Kendy Charleswilkendy80@gmail.com"/>
-    <hyperlink ref="D223" r:id="rId141" display="mariellewilniamoise@gmail.com"/>
-    <hyperlink ref="D224" r:id="rId142" display="ginnesoneseide@gmail.com"/>
-    <hyperlink ref="D225" r:id="rId143" display="altanasrodney@gmail.com"/>
-    <hyperlink ref="E225" r:id="rId144" display="Altanas Rodney altanasrodney@gmail.com "/>
-    <hyperlink ref="D226" r:id="rId145" display="jeannotamisi8@gmail.com"/>
-    <hyperlink ref="E226" r:id="rId146" display="Kuzinda Amisi, jeannotamisi8@gmail.com"/>
-    <hyperlink ref="D227" r:id="rId147" display="alhadisadill@gmail.com"/>
-    <hyperlink ref="D228" r:id="rId148" display="ISharasafari@gmail.co"/>
-    <hyperlink ref="D229" r:id="rId149" display="espoirkateye@gmail.com"/>
-    <hyperlink ref="D230" r:id="rId150" display="sadikikaskile@gmail.com"/>
-    <hyperlink ref="D231" r:id="rId151" display="shanikekihumbu6@gmail.com"/>
-    <hyperlink ref="D232" r:id="rId152" display="ruzosruzamuka@gmail.com"/>
-    <hyperlink ref="D233" r:id="rId153" display="ruzosruzamuka@gmail.com"/>
-    <hyperlink ref="D234" r:id="rId154" display="jaunathancharlemategera@gmail.com"/>
-    <hyperlink ref="D235" r:id="rId155" display="chantallub063@ail.com"/>
-    <hyperlink ref="D236" r:id="rId156" display="ruzosruzamuka@gmail.com"/>
-    <hyperlink ref="D237" r:id="rId157" display="ropoomodoman@gmail.com"/>
-    <hyperlink ref="D238" r:id="rId158" display="georgeolihafrancis52@gmail.com"/>
-    <hyperlink ref="D239" r:id="rId159" display="esthertuna12@gmail.com"/>
-    <hyperlink ref="D240" r:id="rId160" display="perinamatthew3@gmail.com"/>
-    <hyperlink ref="D241" r:id="rId161" display="dominiclojore1@gmail.com"/>
-    <hyperlink ref="D242" r:id="rId162" display="bettyjokudu92@gmail.com"/>
-    <hyperlink ref="D243" r:id="rId163" display="cigunduchristophajeanclaude@gail.com"/>
-    <hyperlink ref="D244" r:id="rId164" display="akunyajake@gmail.com"/>
-    <hyperlink ref="D245" r:id="rId165" display="graceituba242@gmail.com"/>
-    <hyperlink ref="D246" r:id="rId166" display="lokikorokjames@glail.com"/>
-    <hyperlink ref="D247" r:id="rId167" display="marynightjames@gmail.com"/>
-    <hyperlink ref="D248" r:id="rId168" display="prizeemmanuel45@gmail.com"/>
-    <hyperlink ref="D249" r:id="rId169" display="kelijobwoy@gmail.com"/>
-    <hyperlink ref="D250" r:id="rId170" display="ahicherjohnmarkdachi01@gmzik.com"/>
-    <hyperlink ref="D251" r:id="rId171" display="zolienferidafaisal@gmzil.com"/>
-    <hyperlink ref="D252" r:id="rId172" display="jamessaga36@gmail.com"/>
-    <hyperlink ref="D253" r:id="rId173" display="ndayisabac985@gmail.com"/>
-    <hyperlink ref="D254" r:id="rId174" display="iradukundajosias04@gmail.com"/>
-    <hyperlink ref="D255" r:id="rId175" display="bahatibavurikivalery@gmail.com"/>
-    <hyperlink ref="D256" r:id="rId176" display="sindayigayaatanase@gmai.com"/>
-    <hyperlink ref="D257" r:id="rId177" display="sibomanajeanpierre@gmail.com"/>
-    <hyperlink ref="D258" r:id="rId178" display="kwizerajeanmarie54@gmail.com"/>
-    <hyperlink ref="D259" r:id="rId179" display="lobalujames09@gmail.com"/>
-    <hyperlink ref="D260" r:id="rId180" display="jamesladulokang@gmail.com"/>
-    <hyperlink ref="D261" r:id="rId181" display="Nyabaribo@gmail.com"/>
-    <hyperlink ref="D262" r:id="rId182" display="susanono881@mail.com"/>
-    <hyperlink ref="D263" r:id="rId183" display="gabrielatahu13@gmail.com"/>
-    <hyperlink ref="D264" r:id="rId184" display="dominicohisa766@gmail.com"/>
-    <hyperlink ref="D265" r:id="rId185" display="yasinisick@glail.com"/>
-    <hyperlink ref="D266" r:id="rId186" display="derarachobang12@gmail.com"/>
-    <hyperlink ref="D267" r:id="rId187" display="johnoting065@gmail.com"/>
-    <hyperlink ref="D268" r:id="rId188" display="ladusimon166@gmail.com"/>
-    <hyperlink ref="D269" r:id="rId189" display="marangoobuy97@gmail.com"/>
-    <hyperlink ref="D270" r:id="rId190" display="obangojullu900@gmail.com"/>
-    <hyperlink ref="D271" r:id="rId191" display="amanimufing@gmail.com"/>
-    <hyperlink ref="D272" r:id="rId192" display="deborakashindi@gmail.com"/>
-    <hyperlink ref="D273" r:id="rId193" display="rbalebanga@gmail.com"/>
-    <hyperlink ref="E273" r:id="rId194" display=" RamazaniBalebanga    rbalebanga@gmail.com"/>
-    <hyperlink ref="D274" r:id="rId195" display="yakobobalibuzajacques@gmail.com"/>
-    <hyperlink ref="E274" r:id="rId196" display="Balibuza jacques, yakobobalibuzajacques@gmail.com"/>
-    <hyperlink ref="D275" r:id="rId197" display="kyatokekwamoise@gmail.com"/>
-    <hyperlink ref="D276" r:id="rId198" display="shukurumashalialfred@gmail.com"/>
-    <hyperlink ref="D277" r:id="rId199" display="samuelchikwanine69@gmail.com"/>
-    <hyperlink ref="D278" r:id="rId200" display="cmushoshere@gmail.com"/>
-    <hyperlink ref="D279" r:id="rId201" display="balamilwangila@gmail.com"/>
-    <hyperlink ref="D280" r:id="rId202" display="niwamunguarcen@gmail.com"/>
-    <hyperlink ref="D281" r:id="rId203" display="bahatikalangiro@gmail.com"/>
-    <hyperlink ref="D282" r:id="rId204" display="johnnzanzu55@gmail.com"/>
-    <hyperlink ref="D283" r:id="rId205" display="buchiza2019@gmail.com"/>
-    <hyperlink ref="E283" r:id="rId206" display="buchiza2019@gmail.com"/>
-    <hyperlink ref="D284" r:id="rId207" display="mbalapatrick054@gmail.com"/>
-    <hyperlink ref="E284" r:id="rId208" display="Patrick mbala mbalapatrick054@gmail.com"/>
-    <hyperlink ref="D285" r:id="rId209" display="jacksonmapendo2022@gmail.com"/>
-    <hyperlink ref="E285" r:id="rId210" display="Nom: Mapendo Jackson. Adresse e-mail: jacksonmapendo2022@gmail.com"/>
-    <hyperlink ref="D286" r:id="rId211" display="confortieca@gmail.com"/>
-    <hyperlink ref="D287" r:id="rId212" display="mosesnadogera@gmail.com"/>
-    <hyperlink ref="D288" r:id="rId213" display="AmosMuba@gmail.com"/>
-    <hyperlink ref="D289" r:id="rId214" display="esthertereza@gmail.com"/>
-    <hyperlink ref="D290" r:id="rId215" display="clovisrashid@gmail.com"/>
-    <hyperlink ref="D291" r:id="rId216" display="kizakatunda@gmail.com"/>
-    <hyperlink ref="D292" r:id="rId217" display="bisimwakiza@gmail.com"/>
-    <hyperlink ref="D293" r:id="rId218" display="zihalirwachanel@gmail.com"/>
-    <hyperlink ref="D294" r:id="rId219" display="kenembokismbira@gmail.com"/>
-    <hyperlink ref="D295" r:id="rId220" display="chizungunoela@gmail.com"/>
-    <hyperlink ref="D296" r:id="rId221" display="moshihuseni@gmail.com"/>
-    <hyperlink ref="D297" r:id="rId222" display="kakoziamidu@gmail.com"/>
-    <hyperlink ref="D298" r:id="rId223" display="nzabimanaprotais@gmail.com"/>
-    <hyperlink ref="D299" r:id="rId224" display="stevenchristiansumbestevenchri@gmail.com"/>
-    <hyperlink ref="D300" r:id="rId225" display="poepoleclaude5@gmail.com"/>
-    <hyperlink ref="D301" r:id="rId226" display="bahatimunyakazi@gmail.com"/>
-    <hyperlink ref="D302" r:id="rId227" display="sylvestrebazabishaka@gmal.icom"/>
-    <hyperlink ref="D303" r:id="rId228" display="simonkoko097@gmail.com"/>
-    <hyperlink ref="D304" r:id="rId229" display="imaniyleo@gmail.com"/>
-    <hyperlink ref="D305" r:id="rId230" display="amisibernadette21@gmail.com"/>
-    <hyperlink ref="D306" r:id="rId231" display="madoyafeti@mail.com"/>
-    <hyperlink ref="D307" r:id="rId232" display="eritieilondelo@gmail.com"/>
-    <hyperlink ref="D308" r:id="rId233" display="alicemukucha@gmail.com"/>
-    <hyperlink ref="D309" r:id="rId234" display="niwamungubalaguzi@gmail.com"/>
-    <hyperlink ref="D310" r:id="rId235" display="arthemassoroba@gmail.com"/>
-    <hyperlink ref="D311" r:id="rId236" display="cead4408@gmail.com"/>
-    <hyperlink ref="D312" r:id="rId237" display="fanonerantsoaf@gmail.com"/>
-    <hyperlink ref="D313" r:id="rId238" display="fehiniaina09@gmail.com"/>
-    <hyperlink ref="D314" r:id="rId239" display="irandrianaryjames@gmail.com"/>
-    <hyperlink ref="D315" r:id="rId240" display="maheryandria050@gmail.com"/>
-    <hyperlink ref="D316" r:id="rId241" display="donissafenotiana@gmail.com"/>
-    <hyperlink ref="D317" r:id="rId242" display="felanantsoa5@gmail.com"/>
-    <hyperlink ref="D318" r:id="rId243" display="bidybidy326@gmail.com"/>
-    <hyperlink ref="D319" r:id="rId244" display="anjamichya@gmail.com"/>
-    <hyperlink ref="D320" r:id="rId245" display="Hariniainasynie@gmail.com"/>
-    <hyperlink ref="D321" r:id="rId246" display="rakotoarisoloe@gmail.com"/>
-    <hyperlink ref="D322" r:id="rId247" display="maminirinaandrianjanaka@gmail.com"/>
-    <hyperlink ref="D323" r:id="rId248" display="anjaraheridio@gmail.com"/>
-    <hyperlink ref="D324" r:id="rId249" display="tonyrazaf111@gmail.com"/>
-    <hyperlink ref="D325" r:id="rId250" display="andritianamickaelrak0102@gmail.com"/>
-    <hyperlink ref="D326" r:id="rId251" display="razakanirinafeno@gmail.com"/>
-    <hyperlink ref="D327" r:id="rId252" display="rjniainarinah@gmail.com"/>
-    <hyperlink ref="D328" r:id="rId253" display="franciarmf0@gmail.com"/>
-    <hyperlink ref="D329" r:id="rId254" display="aronekenarak@gmail.com"/>
-    <hyperlink ref="D330" r:id="rId255" display="andrianjaka127@gmail.com"/>
-    <hyperlink ref="D331" r:id="rId256" display="raharimalalaedminah@gmail.com"/>
-    <hyperlink ref="D332" r:id="rId257" display="jeremie2004jeremie@gmail.com"/>
-    <hyperlink ref="D333" r:id="rId258" display="lanjaniainaherizo@gmail.com"/>
-    <hyperlink ref="D334" r:id="rId259" display="rijaniainarafanomezantsoa@gmail.com"/>
-    <hyperlink ref="D335" r:id="rId260" display="fanjavanaharintsoa@gmail.com"/>
-    <hyperlink ref="D336" r:id="rId261" display="priscarazafimah@gmail.com"/>
-    <hyperlink ref="D337" r:id="rId262" display="raharimalalatojo5@gmail.com"/>
-    <hyperlink ref="D338" r:id="rId263" display="berthelivamarizony@gmail.com"/>
-    <hyperlink ref="D339" r:id="rId264" display="fanambinantsoasedera2005@gmail.com"/>
-    <hyperlink ref="D340" r:id="rId265" display="nandrasaniaina@gmail.com"/>
-    <hyperlink ref="D341" r:id="rId266" display="synedrionar@gmail.com"/>
-    <hyperlink ref="D342" r:id="rId267" display="tahiry2210@gmail.com"/>
-    <hyperlink ref="D343" r:id="rId268" display="Sandriicah@gmail.com"/>
-    <hyperlink ref="D344" r:id="rId269" display="ra.samydondieu@gmail.com"/>
-    <hyperlink ref="D345" r:id="rId270" display="miantsahanitriniala33@gmail.com"/>
-    <hyperlink ref="D346" r:id="rId271" display="mialyharimanana30@gmail.com"/>
-    <hyperlink ref="D347" r:id="rId272" display="nyaina21.aps2b@gmail.com"/>
-    <hyperlink ref="D348" r:id="rId273" display="sandriicah@gmail.com"/>
-    <hyperlink ref="D349" r:id="rId274" display="nirinamonirah04@gmail.com"/>
-    <hyperlink ref="D350" r:id="rId275" display="zoelinahralaivoavy@gmail.com"/>
-    <hyperlink ref="D351" r:id="rId276" display="rakotondrabaryfano@gmail.com"/>
-    <hyperlink ref="D352" r:id="rId277" display="tsinjosantatra@gmail.com"/>
-    <hyperlink ref="D353" r:id="rId278" display="fehizoromamenosoa@gmail.com"/>
-    <hyperlink ref="D354" r:id="rId279" display="nomenjanahary.francia.noum@gmail.com"/>
-    <hyperlink ref="D355" r:id="rId280" display="priscarazafimah@gmail.com"/>
-    <hyperlink ref="D356" r:id="rId281" display="jessicaraharinirina17@gmail.com"/>
-    <hyperlink ref="D357" r:id="rId282" display="rafalimananajunior7@gmail.com"/>
-    <hyperlink ref="D358" r:id="rId283" display="nambinintsolaza@gmail.com"/>
-    <hyperlink ref="D359" r:id="rId284" display="narindraandrianjanaka@gmail.com"/>
-    <hyperlink ref="D360" r:id="rId285" display="fitiavanacynthia090@gmail.com"/>
-    <hyperlink ref="D361" r:id="rId286" display="fanangama2@gmail.com"/>
-    <hyperlink ref="D362" r:id="rId287" display="randriamparanynomena49@gmail.com"/>
-    <hyperlink ref="D363" r:id="rId288" display="andrianjaka127@gmail.com"/>
-    <hyperlink ref="D364" r:id="rId289" display="ratsimanohatrarado@gmail.com"/>
-    <hyperlink ref="D365" r:id="rId290" display="andriatoky132@gmail.com"/>
-    <hyperlink ref="D366" r:id="rId291" display="mayarantonirina@gmail.com"/>
-    <hyperlink ref="D367" r:id="rId292" display="haingonathie@gmail.com"/>
-    <hyperlink ref="D368" r:id="rId293" display="rafanambinantsoastephanie@gmail.com"/>
-    <hyperlink ref="D369" r:id="rId294" display="andrialivah2@gmail.com"/>
-    <hyperlink ref="D370" r:id="rId295" display="randrianantenainalazatian@gmail.com"/>
-    <hyperlink ref="D371" r:id="rId296" display="rakotomalalavictoria3@gmail.com"/>
-    <hyperlink ref="D372" r:id="rId297" display="sandymamitiana6@gmail.com"/>
-    <hyperlink ref="D373" r:id="rId298" display="stephanierasoafaniry4@gmail.com"/>
-    <hyperlink ref="D374" r:id="rId299" display="jimmyerving594@gmail.com"/>
-    <hyperlink ref="D375" r:id="rId300" display="miharisoanancia3@gmail.com"/>
-    <hyperlink ref="D376" r:id="rId301" display="razafimananamolisco@gmail.com"/>
-    <hyperlink ref="D377" r:id="rId302" display="ramilijohn@gmail.com"/>
-    <hyperlink ref="D378" r:id="rId303" display="elysafanirisoa@gmail.com"/>
-    <hyperlink ref="D379" r:id="rId304" display="raharinambininanekena@gmail.com"/>
-    <hyperlink ref="D380" r:id="rId305" display="tsiryezeckiel@gmail.com"/>
-    <hyperlink ref="D381" r:id="rId306" display="noummiandry@gmail.com"/>
-    <hyperlink ref="D382" r:id="rId307" display="aravonavalona@gmail.com"/>
-    <hyperlink ref="D383" r:id="rId308" display="artinetteheryvololona@gmail.com"/>
-    <hyperlink ref="D384" r:id="rId309" display="manampisoafandresenaa@gmail.com"/>
-    <hyperlink ref="D385" r:id="rId310" display="Mallsafidy913@gmail.com"/>
-    <hyperlink ref="D386" r:id="rId311" display="Fiafaranafiafarana@gmail.com"/>
-    <hyperlink ref="D387" r:id="rId312" display="tokyandrianarivo601@gmail.com"/>
-    <hyperlink ref="D388" r:id="rId313" display="nisokoxeno@gmail.com"/>
-    <hyperlink ref="D389" r:id="rId314" display="minorakoto32@gmail.com"/>
-    <hyperlink ref="D390" r:id="rId315" display="Gasikara42@gmail.com"/>
-    <hyperlink ref="D391" r:id="rId316" display="fanevaf47@gmail.com"/>
-    <hyperlink ref="D392" r:id="rId317" display="solofoharilalahernola@gmail.com"/>
-    <hyperlink ref="D393" r:id="rId318" display="rakotonirinamanda977@gmail.com"/>
-    <hyperlink ref="D394" r:id="rId319" display="Tinamandimbiarivo@gmail.com"/>
-    <hyperlink ref="D395" r:id="rId320" display="Stephanieraharison13@gmail.com"/>
-    <hyperlink ref="D396" r:id="rId321" display="voahariniaina117@gmail.com"/>
-    <hyperlink ref="D397" r:id="rId322" display="raisaserge1001@gmail.com"/>
-    <hyperlink ref="D398" r:id="rId323" display="ChandrineRahariniony@gmail.com"/>
-    <hyperlink ref="D399" r:id="rId324" display="rfttoussaint@gmail.com"/>
-    <hyperlink ref="D400" r:id="rId325" display="lovasoaraharimalala1@gmail.com"/>
-    <hyperlink ref="D401" r:id="rId326" display="nahfahatsiarovana@gmail.com"/>
-    <hyperlink ref="D402" r:id="rId327" display="onjacomrakoto@gmail.com"/>
-    <hyperlink ref="D403" r:id="rId328" display="ravomahefa2603@gmail.com"/>
-    <hyperlink ref="D404" r:id="rId329" display="zoly.raholinirina@gmail.com"/>
-    <hyperlink ref="D405" r:id="rId330" display="nalyravalison@gmail.com"/>
-    <hyperlink ref="D406" r:id="rId331" display="fifalianaandriamiravo@gmail.com"/>
-    <hyperlink ref="D407" r:id="rId332" display="hasinalalainarazafindrakoto@gmail.com"/>
-    <hyperlink ref="D408" r:id="rId333" display="Kiadyrandriamaharison@gmail.com"/>
-    <hyperlink ref="D409" r:id="rId334" display="alphonse.jean5236@gmail.com"/>
-    <hyperlink ref="D410" r:id="rId335" display="andonirinaraharimbalimiorantso@gmail.com"/>
-    <hyperlink ref="D411" r:id="rId336" display="dinanantenaina05@gmail.com"/>
-    <hyperlink ref="D412" r:id="rId337" display="miorarvk@gmail.com"/>
-    <hyperlink ref="D413" r:id="rId338" display="ebida912@gmail.com"/>
-    <hyperlink ref="E413" r:id="rId339" display="ebida912@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId3" display="yakobobalibuzajacques@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId4" display="kitumainimakeledeodate@gmail.com"/>
+    <hyperlink ref="D7" r:id="rId5" display="nondamulenga@gamil.com"/>
+    <hyperlink ref="D8" r:id="rId6" display="shimazephy6@gmail.com"/>
+    <hyperlink ref="D9" r:id="rId7" display="Agroanzuruni@gmail.com"/>
+    <hyperlink ref="D10" r:id="rId8" display="iragijeff@gmail.com"/>
+    <hyperlink ref="D11" r:id="rId9" display="kwizerajeanmarie53@gmail.com"/>
+    <hyperlink ref="D12" r:id="rId10" display="triomphebirenganya@gmail.om"/>
+    <hyperlink ref="D13" r:id="rId11" display="ausengimanaodette34@gmail.com"/>
+    <hyperlink ref="AI13" r:id="rId12" display="Le plus difficile, c’est de ne pas pouvoir transmettre l’émotion ou l’intention exacte ça peut créer des malentendus ou briser la connexion.si le sujet est Mal étendu &#10;"/>
+    <hyperlink ref="D14" r:id="rId13" display="cimushoshere@gmail.com"/>
+    <hyperlink ref="D15" r:id="rId14" display="eddymulindwa013@gmail.com"/>
+    <hyperlink ref="D16" r:id="rId15" display="bizimanajuvenal@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId16" display="conforgeca@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId17" display="jacquesbahati37@gmail.com"/>
+    <hyperlink ref="D19" r:id="rId18" display="denismunguiko12@gmail.com"/>
+    <hyperlink ref="D20" r:id="rId19" display="hopevisioneenterprise@gmail.com"/>
+    <hyperlink ref="D21" r:id="rId20" display="bahatikalangirosamuel@gmail.com"/>
+    <hyperlink ref="D22" r:id="rId21" display="benjaminngota@gmail.com"/>
+    <hyperlink ref="D23" r:id="rId22" display="kipondaruvukisha@gmail.com"/>
+    <hyperlink ref="D24" r:id="rId23" display="mauwaizakiena@gmail.com"/>
+    <hyperlink ref="D25" r:id="rId24" display="irandukundafleury@gmail.com"/>
+    <hyperlink ref="D26" r:id="rId25" display="uwizeyimanapaskarine@gmail.com"/>
+    <hyperlink ref="D27" r:id="rId26" display="mugishablaise961@gmail.com"/>
+    <hyperlink ref="D28" r:id="rId27" display="herietteliwilana@gmail.com"/>
+    <hyperlink ref="D29" r:id="rId28" display="vanessashimirimana@gmail.com"/>
+    <hyperlink ref="D30" r:id="rId29" display="imaniyaleoboutros2@gmail.com"/>
+    <hyperlink ref="D31" r:id="rId30" display="winvestine@gmail.com"/>
+    <hyperlink ref="D32" r:id="rId31" display="katingwamasanzeleo@gmail.com"/>
+    <hyperlink ref="D33" r:id="rId32" display="Innocentuwezosebareka@gamil.com"/>
+    <hyperlink ref="D34" r:id="rId33" display="Barakasebaraka@gmail.com"/>
+    <hyperlink ref="D35" r:id="rId34" display="kingjacksonmuleka@gmail.com"/>
+    <hyperlink ref="D36" r:id="rId35" display="johnmunguiko643@gmqil.com"/>
+    <hyperlink ref="D37" r:id="rId36" display="Naimasumami@gmail.com"/>
+    <hyperlink ref="D38" r:id="rId37" display="shabanikaffifa@gmail.com"/>
+    <hyperlink ref="D39" r:id="rId38" display="Akimanakelly@gmail.com"/>
+    <hyperlink ref="D40" r:id="rId39" display="Nyandubonybonny@gmail.com"/>
+    <hyperlink ref="D41" r:id="rId40" display="achizajeff@gmail.com"/>
+    <hyperlink ref="D42" r:id="rId41" display="clovisrashidi457@gmail.com"/>
+    <hyperlink ref="D43" r:id="rId42" display="somodtwagira@gmail.com"/>
+    <hyperlink ref="D44" r:id="rId43" display="Nadegendwangayesu@gmail.com"/>
+    <hyperlink ref="D45" r:id="rId44" display="gowingongwe@gmail.com"/>
+    <hyperlink ref="D46" r:id="rId45" display="misumbamitunga@gmail.com"/>
+    <hyperlink ref="D47" r:id="rId46" display="marcelinemungama@gmail.com"/>
+    <hyperlink ref="D48" r:id="rId47" display="Luson6@gmil.com"/>
+    <hyperlink ref="D49" r:id="rId48" display="mwaminichristel@gmail.com"/>
+    <hyperlink ref="D50" r:id="rId49" display="fistonbikuku@gmail.com"/>
+    <hyperlink ref="D51" r:id="rId50" display="mugishablaise961@gmail.com"/>
+    <hyperlink ref="D52" r:id="rId51" display="niwamungubalazi@gmail.com"/>
+    <hyperlink ref="D53" r:id="rId52" display="fifiviane@gmail.com"/>
+    <hyperlink ref="D54" r:id="rId53" display="joycemanirakiza6@gmail.com"/>
+    <hyperlink ref="D55" r:id="rId54" display="abwemkyombwechristophe@gmail.com"/>
+    <hyperlink ref="D56" r:id="rId55" display="shanikehonda6@gmail.com"/>
+    <hyperlink ref="D57" r:id="rId56" display="irakundeliesse@gmail.com"/>
+    <hyperlink ref="D58" r:id="rId57" display="hayarimanaclairia@gmail.com"/>
+    <hyperlink ref="D59" r:id="rId58" display="habiyambeemmanuel@gail.com"/>
+    <hyperlink ref="D60" r:id="rId59" display="espoirkalamo@gmail.com"/>
+    <hyperlink ref="D61" r:id="rId60" display="somodtwagira@gmail.com"/>
+    <hyperlink ref="D62" r:id="rId61" display="ernestmikato@gmail.com"/>
+    <hyperlink ref="D63" r:id="rId62" display="abrahamod@gmail.com"/>
+    <hyperlink ref="D64" r:id="rId63" display="kipondaruvukisha@gmail.com"/>
+    <hyperlink ref="D65" r:id="rId64" display="muzaliwarashidi93@gmail.com"/>
+    <hyperlink ref="D66" r:id="rId65" display="azizamwabwa@gmail.com"/>
+    <hyperlink ref="D67" r:id="rId66" display="fikiriwafikiri@gmail.com"/>
+    <hyperlink ref="D68" r:id="rId67" display="albertalka@gmail.com"/>
+    <hyperlink ref="D69" r:id="rId68" display="apolinaanna@gmail.com"/>
+    <hyperlink ref="D70" r:id="rId69" display="bisimwaciza387@gmail.com"/>
+    <hyperlink ref="D71" r:id="rId70" display="blaisebitangimana18@gmail.com"/>
+    <hyperlink ref="D72" r:id="rId71" display="bonynyandu@gmail.com"/>
+    <hyperlink ref="D73" r:id="rId72" display="cadeaungakani@gmail.com"/>
+    <hyperlink ref="D74" r:id="rId73" display="christellemwamini026@gmail.com"/>
+    <hyperlink ref="D75" r:id="rId74" display="cizaladent@gmail.com"/>
+    <hyperlink ref="D76" r:id="rId75" display="davidblessingjanvier@gmail.com"/>
+    <hyperlink ref="D77" r:id="rId76" display="delphinwingimana8@gmail.com"/>
+    <hyperlink ref="D78" r:id="rId77" display="dusabejisele@gmail.com"/>
+    <hyperlink ref="D79" r:id="rId78" display="dusengimanaodette34@gmail.com"/>
+    <hyperlink ref="D80" r:id="rId79" display="faidabimule@gmail.com"/>
+    <hyperlink ref="D81" r:id="rId80" display="fifiviane@gmail.com"/>
+    <hyperlink ref="D82" r:id="rId81" display="fikiriwafikiri@gmail.com"/>
+    <hyperlink ref="D83" r:id="rId82" display="gilbermukacho@gmail.com"/>
+    <hyperlink ref="D84" r:id="rId83" display="hayarimanaclairia@gmail.com"/>
+    <hyperlink ref="D85" r:id="rId84" display="ibrahimramazani@gmail.com"/>
+    <hyperlink ref="D86" r:id="rId85" display="kalamuespoire35@gmail.com"/>
+    <hyperlink ref="D87" r:id="rId86" display="kennygakwanya7@gmail.com"/>
+    <hyperlink ref="D88" r:id="rId87" display="kingnikolasngakani@gmail.com"/>
+    <hyperlink ref="D89" r:id="rId88" display="kwizerajeanmarie53@gmail.com"/>
+    <hyperlink ref="D90" r:id="rId89" display="mavukojohnbosco@gmail.com"/>
+    <hyperlink ref="D91" r:id="rId90" display="mosesnandogera@gmail.com"/>
+    <hyperlink ref="D92" r:id="rId91" display="mubaamos5@gmail.com"/>
+    <hyperlink ref="D93" r:id="rId92" display="mugishaabdulakarim48@gmail.com"/>
+    <hyperlink ref="D94" r:id="rId93" display="nduwimanadesire449@gmail.com"/>
+    <hyperlink ref="E94" r:id="rId94" display="nduwimanadesire449@gmail.com"/>
+    <hyperlink ref="D95" r:id="rId95" display="nishimwehassan@gmail.com"/>
+    <hyperlink ref="D96" r:id="rId96" display="ebuelayamungu@gmail.com"/>
+    <hyperlink ref="D97" r:id="rId97" display="josephjilardo@gmail.com"/>
+    <hyperlink ref="D98" r:id="rId98" display="januarybessinesjile@gmail.com"/>
+    <hyperlink ref="D99" r:id="rId99" display="farijikalukuli@gmail.com"/>
+    <hyperlink ref="D100" r:id="rId100" display="fidelematete@gmail.com"/>
+    <hyperlink ref="D101" r:id="rId101" display="kivulibko7@gmail.com"/>
+    <hyperlink ref="D102" r:id="rId102" display="juniormekhan60@gmail.com"/>
+    <hyperlink ref="D103" r:id="rId103" display="oscarmusabimana4@gmail.co"/>
+    <hyperlink ref="D104" r:id="rId104" display="mavulano5@gmail.com"/>
+    <hyperlink ref="D105" r:id="rId105" display="apendkieresi@gmail.com"/>
+    <hyperlink ref="D106" r:id="rId106" display="angelolokorai@gmail.com"/>
+    <hyperlink ref="D107" r:id="rId107" display="kwalibbko7@gmail.com"/>
+    <hyperlink ref="D108" r:id="rId108" display="mulenganonda1@gmail.com"/>
+    <hyperlink ref="D109" r:id="rId109" display="mugishaabdulakarim487@gmail.com"/>
+    <hyperlink ref="D110" r:id="rId110" display="tomthree190@gmail.com"/>
+    <hyperlink ref="D111" r:id="rId111" display="vincentnduwamungu48@gmail.com"/>
+    <hyperlink ref="D112" r:id="rId112" display="pacificnundu@gmail.com"/>
+    <hyperlink ref="D113" r:id="rId113" display="zainaswedi9@gmail.com"/>
+    <hyperlink ref="D114" r:id="rId114" display="wasalumiwasalumu@gmail.com"/>
+    <hyperlink ref="D115" r:id="rId115" display="olivier4@gmail.com"/>
+    <hyperlink ref="D116" r:id="rId116" display="achizajeff@gmail.com"/>
+    <hyperlink ref="D117" r:id="rId117" display="juniormekhan60@gmail.com"/>
+    <hyperlink ref="D118" r:id="rId118" display="alka01139@gmail.com"/>
+    <hyperlink ref="D119" r:id="rId119" display="f81925614@gmail.com"/>
+    <hyperlink ref="D120" r:id="rId120" display="apendkieresi@gmail.com"/>
+    <hyperlink ref="D121" r:id="rId121" display="chizabisimwa5@gmail.com"/>
+    <hyperlink ref="D122" r:id="rId122" display="angelolokorai@gmail.com"/>
+    <hyperlink ref="D123" r:id="rId123" display="imaniyaleoboutros2@gmail.com"/>
+    <hyperlink ref="D124" r:id="rId124" display="kivulibk07@gmail.com"/>
+    <hyperlink ref="D125" r:id="rId125" display="cholvalentines737@gmail.com"/>
+    <hyperlink ref="D126" r:id="rId126" display="meshefaustin@gmail.com"/>
+    <hyperlink ref="D127" r:id="rId127" display="mwaminichimanuka@gmail.com"/>
+    <hyperlink ref="D128" r:id="rId128" display="kwalibbko7@gmail.com"/>
+    <hyperlink ref="D129" r:id="rId129" display="kichonavenuelle@gmail.com"/>
+    <hyperlink ref="D130" r:id="rId130" display="stephenokech@gmail.com"/>
+    <hyperlink ref="D131" r:id="rId131" display="bizimanajuvenel120@gmail.com"/>
+    <hyperlink ref="D218" r:id="rId132" display="desirjeanedens75@gmail.com"/>
+    <hyperlink ref="D219" r:id="rId133" display="sandra.jean2@icloud.com"/>
+    <hyperlink ref="D220" r:id="rId134" display="davidjeanpierre772@gmail.com"/>
+    <hyperlink ref="D221" r:id="rId135" display="prospereedno27@gmail.com"/>
+    <hyperlink ref="D222" r:id="rId136" display="charleswilkendy80@gmail.com"/>
+    <hyperlink ref="E222" r:id="rId137" display="Kendy Charleswilkendy80@gmail.com"/>
+    <hyperlink ref="D223" r:id="rId138" display="mariellewilniamoise@gmail.com"/>
+    <hyperlink ref="D224" r:id="rId139" display="ginnesoneseide@gmail.com"/>
+    <hyperlink ref="D225" r:id="rId140" display="altanasrodney@gmail.com"/>
+    <hyperlink ref="D226" r:id="rId141" display="jeannotamisi8@gmail.com"/>
+    <hyperlink ref="D227" r:id="rId142" display="alhadisadill@gmail.com"/>
+    <hyperlink ref="D228" r:id="rId143" display="ISharasafari@gmail.co"/>
+    <hyperlink ref="D229" r:id="rId144" display="espoirkateye@gmail.com"/>
+    <hyperlink ref="D230" r:id="rId145" display="sadikikaskile@gmail.com"/>
+    <hyperlink ref="D231" r:id="rId146" display="shanikekihumbu6@gmail.com"/>
+    <hyperlink ref="D232" r:id="rId147" display="ruzosruzamuka@gmail.com"/>
+    <hyperlink ref="D233" r:id="rId148" display="ruzosruzamuka@gmail.com"/>
+    <hyperlink ref="D234" r:id="rId149" display="jaunathancharlemategera@gmail.com"/>
+    <hyperlink ref="D235" r:id="rId150" display="chantallub063@ail.com"/>
+    <hyperlink ref="D236" r:id="rId151" display="ruzosruzamuka@gmail.com"/>
+    <hyperlink ref="D237" r:id="rId152" display="ropoomodoman@gmail.com"/>
+    <hyperlink ref="D238" r:id="rId153" display="georgeolihafrancis52@gmail.com"/>
+    <hyperlink ref="D239" r:id="rId154" display="esthertuna12@gmail.com"/>
+    <hyperlink ref="D240" r:id="rId155" display="perinamatthew3@gmail.com"/>
+    <hyperlink ref="D241" r:id="rId156" display="dominiclojore1@gmail.com"/>
+    <hyperlink ref="D242" r:id="rId157" display="bettyjokudu92@gmail.com"/>
+    <hyperlink ref="D243" r:id="rId158" display="cigunduchristophajeanclaude@gail.com"/>
+    <hyperlink ref="D244" r:id="rId159" display="akunyajake@gmail.com"/>
+    <hyperlink ref="D245" r:id="rId160" display="graceituba242@gmail.com"/>
+    <hyperlink ref="D246" r:id="rId161" display="lokikorokjames@glail.com"/>
+    <hyperlink ref="D247" r:id="rId162" display="marynightjames@gmail.com"/>
+    <hyperlink ref="D248" r:id="rId163" display="prizeemmanuel45@gmail.com"/>
+    <hyperlink ref="D249" r:id="rId164" display="kelijobwoy@gmail.com"/>
+    <hyperlink ref="D250" r:id="rId165" display="ahicherjohnmarkdachi01@gmzik.com"/>
+    <hyperlink ref="D251" r:id="rId166" display="zolienferidafaisal@gmzil.com"/>
+    <hyperlink ref="D252" r:id="rId167" display="jamessaga36@gmail.com"/>
+    <hyperlink ref="D253" r:id="rId168" display="ndayisabac985@gmail.com"/>
+    <hyperlink ref="D254" r:id="rId169" display="iradukundajosias04@gmail.com"/>
+    <hyperlink ref="D255" r:id="rId170" display="bahatibavurikivalery@gmail.com"/>
+    <hyperlink ref="D256" r:id="rId171" display="sindayigayaatanase@gmai.com"/>
+    <hyperlink ref="D257" r:id="rId172" display="sibomanajeanpierre@gmail.com"/>
+    <hyperlink ref="D258" r:id="rId173" display="kwizerajeanmarie54@gmail.com"/>
+    <hyperlink ref="D259" r:id="rId174" display="lobalujames09@gmail.com"/>
+    <hyperlink ref="D260" r:id="rId175" display="jamesladulokang@gmail.com"/>
+    <hyperlink ref="D261" r:id="rId176" display="Nyabaribo@gmail.com"/>
+    <hyperlink ref="D262" r:id="rId177" display="susanono881@mail.com"/>
+    <hyperlink ref="D263" r:id="rId178" display="gabrielatahu13@gmail.com"/>
+    <hyperlink ref="D264" r:id="rId179" display="dominicohisa766@gmail.com"/>
+    <hyperlink ref="D265" r:id="rId180" display="yasinisick@glail.com"/>
+    <hyperlink ref="D266" r:id="rId181" display="derarachobang12@gmail.com"/>
+    <hyperlink ref="D267" r:id="rId182" display="johnoting065@gmail.com"/>
+    <hyperlink ref="D268" r:id="rId183" display="ladusimon166@gmail.com"/>
+    <hyperlink ref="D269" r:id="rId184" display="marangoobuy97@gmail.com"/>
+    <hyperlink ref="D270" r:id="rId185" display="obangojullu900@gmail.com"/>
+    <hyperlink ref="D271" r:id="rId186" display="amanimufing@gmail.com"/>
+    <hyperlink ref="D272" r:id="rId187" display="deborakashindi@gmail.com"/>
+    <hyperlink ref="D273" r:id="rId188" display="rbalebanga@gmail.com"/>
+    <hyperlink ref="D274" r:id="rId189" display="yakobobalibuzajacques@gmail.com"/>
+    <hyperlink ref="D275" r:id="rId190" display="kyatokekwamoise@gmail.com"/>
+    <hyperlink ref="D276" r:id="rId191" display="shukurumashalialfred@gmail.com"/>
+    <hyperlink ref="D277" r:id="rId192" display="samuelchikwanine69@gmail.com"/>
+    <hyperlink ref="D278" r:id="rId193" display="cmushoshere@gmail.com"/>
+    <hyperlink ref="D279" r:id="rId194" display="balamilwangila@gmail.com"/>
+    <hyperlink ref="D280" r:id="rId195" display="niwamunguarcen@gmail.com"/>
+    <hyperlink ref="D281" r:id="rId196" display="bahatikalangiro@gmail.com"/>
+    <hyperlink ref="D282" r:id="rId197" display="johnnzanzu55@gmail.com"/>
+    <hyperlink ref="D283" r:id="rId198" display="buchiza2019@gmail.com"/>
+    <hyperlink ref="E283" r:id="rId199" display="buchiza2019@gmail.com"/>
+    <hyperlink ref="D284" r:id="rId200" display="mbalapatrick054@gmail.com"/>
+    <hyperlink ref="D285" r:id="rId201" display="jacksonmapendo2022@gmail.com"/>
+    <hyperlink ref="D286" r:id="rId202" display="confortieca@gmail.com"/>
+    <hyperlink ref="D287" r:id="rId203" display="mosesnadogera@gmail.com"/>
+    <hyperlink ref="D288" r:id="rId204" display="AmosMuba@gmail.com"/>
+    <hyperlink ref="D289" r:id="rId205" display="esthertereza@gmail.com"/>
+    <hyperlink ref="D290" r:id="rId206" display="clovisrashid@gmail.com"/>
+    <hyperlink ref="D291" r:id="rId207" display="kizakatunda@gmail.com"/>
+    <hyperlink ref="D292" r:id="rId208" display="bisimwakiza@gmail.com"/>
+    <hyperlink ref="D293" r:id="rId209" display="zihalirwachanel@gmail.com"/>
+    <hyperlink ref="D294" r:id="rId210" display="kenembokismbira@gmail.com"/>
+    <hyperlink ref="D295" r:id="rId211" display="chizungunoela@gmail.com"/>
+    <hyperlink ref="D296" r:id="rId212" display="moshihuseni@gmail.com"/>
+    <hyperlink ref="D297" r:id="rId213" display="kakoziamidu@gmail.com"/>
+    <hyperlink ref="D298" r:id="rId214" display="nzabimanaprotais@gmail.com"/>
+    <hyperlink ref="D299" r:id="rId215" display="stevenchristiansumbestevenchri@gmail.com"/>
+    <hyperlink ref="D300" r:id="rId216" display="poepoleclaude5@gmail.com"/>
+    <hyperlink ref="D301" r:id="rId217" display="bahatimunyakazi@gmail.com"/>
+    <hyperlink ref="D302" r:id="rId218" display="sylvestrebazabishaka@gmal.icom"/>
+    <hyperlink ref="D303" r:id="rId219" display="simonkoko097@gmail.com"/>
+    <hyperlink ref="D304" r:id="rId220" display="imaniyleo@gmail.com"/>
+    <hyperlink ref="D305" r:id="rId221" display="amisibernadette21@gmail.com"/>
+    <hyperlink ref="D306" r:id="rId222" display="madoyafeti@mail.com"/>
+    <hyperlink ref="D307" r:id="rId223" display="eritieilondelo@gmail.com"/>
+    <hyperlink ref="D308" r:id="rId224" display="alicemukucha@gmail.com"/>
+    <hyperlink ref="D309" r:id="rId225" display="niwamungubalaguzi@gmail.com"/>
+    <hyperlink ref="D310" r:id="rId226" display="arthemassoroba@gmail.com"/>
+    <hyperlink ref="D311" r:id="rId227" display="cead4408@gmail.com"/>
+    <hyperlink ref="D312" r:id="rId228" display="fanonerantsoaf@gmail.com"/>
+    <hyperlink ref="D313" r:id="rId229" display="fehiniaina09@gmail.com"/>
+    <hyperlink ref="D314" r:id="rId230" display="irandrianaryjames@gmail.com"/>
+    <hyperlink ref="D315" r:id="rId231" display="maheryandria050@gmail.com"/>
+    <hyperlink ref="D316" r:id="rId232" display="donissafenotiana@gmail.com"/>
+    <hyperlink ref="D317" r:id="rId233" display="felanantsoa5@gmail.com"/>
+    <hyperlink ref="D318" r:id="rId234" display="bidybidy326@gmail.com"/>
+    <hyperlink ref="D319" r:id="rId235" display="anjamichya@gmail.com"/>
+    <hyperlink ref="D320" r:id="rId236" display="Hariniainasynie@gmail.com"/>
+    <hyperlink ref="D321" r:id="rId237" display="rakotoarisoloe@gmail.com"/>
+    <hyperlink ref="D322" r:id="rId238" display="maminirinaandrianjanaka@gmail.com"/>
+    <hyperlink ref="D323" r:id="rId239" display="anjaraheridio@gmail.com"/>
+    <hyperlink ref="D324" r:id="rId240" display="tonyrazaf111@gmail.com"/>
+    <hyperlink ref="D325" r:id="rId241" display="andritianamickaelrak0102@gmail.com"/>
+    <hyperlink ref="D326" r:id="rId242" display="razakanirinafeno@gmail.com"/>
+    <hyperlink ref="D327" r:id="rId243" display="rjniainarinah@gmail.com"/>
+    <hyperlink ref="D328" r:id="rId244" display="franciarmf0@gmail.com"/>
+    <hyperlink ref="D329" r:id="rId245" display="aronekenarak@gmail.com"/>
+    <hyperlink ref="D330" r:id="rId246" display="andrianjaka127@gmail.com"/>
+    <hyperlink ref="D331" r:id="rId247" display="raharimalalaedminah@gmail.com"/>
+    <hyperlink ref="D332" r:id="rId248" display="jeremie2004jeremie@gmail.com"/>
+    <hyperlink ref="D333" r:id="rId249" display="lanjaniainaherizo@gmail.com"/>
+    <hyperlink ref="D334" r:id="rId250" display="rijaniainarafanomezantsoa@gmail.com"/>
+    <hyperlink ref="D335" r:id="rId251" display="fanjavanaharintsoa@gmail.com"/>
+    <hyperlink ref="D336" r:id="rId252" display="priscarazafimah@gmail.com"/>
+    <hyperlink ref="D337" r:id="rId253" display="raharimalalatojo5@gmail.com"/>
+    <hyperlink ref="D338" r:id="rId254" display="berthelivamarizony@gmail.com"/>
+    <hyperlink ref="D339" r:id="rId255" display="fanambinantsoasedera2005@gmail.com"/>
+    <hyperlink ref="D340" r:id="rId256" display="nandrasaniaina@gmail.com"/>
+    <hyperlink ref="D341" r:id="rId257" display="synedrionar@gmail.com"/>
+    <hyperlink ref="D342" r:id="rId258" display="tahiry2210@gmail.com"/>
+    <hyperlink ref="D343" r:id="rId259" display="Sandriicah@gmail.com"/>
+    <hyperlink ref="D344" r:id="rId260" display="ra.samydondieu@gmail.com"/>
+    <hyperlink ref="D345" r:id="rId261" display="miantsahanitriniala33@gmail.com"/>
+    <hyperlink ref="D346" r:id="rId262" display="mialyharimanana30@gmail.com"/>
+    <hyperlink ref="D347" r:id="rId263" display="nyaina21.aps2b@gmail.com"/>
+    <hyperlink ref="D348" r:id="rId264" display="sandriicah@gmail.com"/>
+    <hyperlink ref="D349" r:id="rId265" display="nirinamonirah04@gmail.com"/>
+    <hyperlink ref="D350" r:id="rId266" display="zoelinahralaivoavy@gmail.com"/>
+    <hyperlink ref="D351" r:id="rId267" display="rakotondrabaryfano@gmail.com"/>
+    <hyperlink ref="D352" r:id="rId268" display="tsinjosantatra@gmail.com"/>
+    <hyperlink ref="D353" r:id="rId269" display="fehizoromamenosoa@gmail.com"/>
+    <hyperlink ref="D354" r:id="rId270" display="nomenjanahary.francia.noum@gmail.com"/>
+    <hyperlink ref="D355" r:id="rId271" display="priscarazafimah@gmail.com"/>
+    <hyperlink ref="D356" r:id="rId272" display="jessicaraharinirina17@gmail.com"/>
+    <hyperlink ref="D357" r:id="rId273" display="rafalimananajunior7@gmail.com"/>
+    <hyperlink ref="D358" r:id="rId274" display="nambinintsolaza@gmail.com"/>
+    <hyperlink ref="D359" r:id="rId275" display="narindraandrianjanaka@gmail.com"/>
+    <hyperlink ref="D360" r:id="rId276" display="fitiavanacynthia090@gmail.com"/>
+    <hyperlink ref="D361" r:id="rId277" display="fanangama2@gmail.com"/>
+    <hyperlink ref="D362" r:id="rId278" display="randriamparanynomena49@gmail.com"/>
+    <hyperlink ref="D363" r:id="rId279" display="andrianjaka127@gmail.com"/>
+    <hyperlink ref="D364" r:id="rId280" display="ratsimanohatrarado@gmail.com"/>
+    <hyperlink ref="D365" r:id="rId281" display="andriatoky132@gmail.com"/>
+    <hyperlink ref="D366" r:id="rId282" display="mayarantonirina@gmail.com"/>
+    <hyperlink ref="D367" r:id="rId283" display="haingonathie@gmail.com"/>
+    <hyperlink ref="D368" r:id="rId284" display="rafanambinantsoastephanie@gmail.com"/>
+    <hyperlink ref="D369" r:id="rId285" display="andrialivah2@gmail.com"/>
+    <hyperlink ref="D370" r:id="rId286" display="randrianantenainalazatian@gmail.com"/>
+    <hyperlink ref="D371" r:id="rId287" display="rakotomalalavictoria3@gmail.com"/>
+    <hyperlink ref="D372" r:id="rId288" display="sandymamitiana6@gmail.com"/>
+    <hyperlink ref="D373" r:id="rId289" display="stephanierasoafaniry4@gmail.com"/>
+    <hyperlink ref="D374" r:id="rId290" display="jimmyerving594@gmail.com"/>
+    <hyperlink ref="D375" r:id="rId291" display="miharisoanancia3@gmail.com"/>
+    <hyperlink ref="D376" r:id="rId292" display="razafimananamolisco@gmail.com"/>
+    <hyperlink ref="D377" r:id="rId293" display="ramilijohn@gmail.com"/>
+    <hyperlink ref="D378" r:id="rId294" display="elysafanirisoa@gmail.com"/>
+    <hyperlink ref="D379" r:id="rId295" display="raharinambininanekena@gmail.com"/>
+    <hyperlink ref="D380" r:id="rId296" display="tsiryezeckiel@gmail.com"/>
+    <hyperlink ref="D381" r:id="rId297" display="noummiandry@gmail.com"/>
+    <hyperlink ref="D382" r:id="rId298" display="aravonavalona@gmail.com"/>
+    <hyperlink ref="D383" r:id="rId299" display="artinetteheryvololona@gmail.com"/>
+    <hyperlink ref="D384" r:id="rId300" display="manampisoafandresenaa@gmail.com"/>
+    <hyperlink ref="D385" r:id="rId301" display="Mallsafidy913@gmail.com"/>
+    <hyperlink ref="D386" r:id="rId302" display="Fiafaranafiafarana@gmail.com"/>
+    <hyperlink ref="D387" r:id="rId303" display="tokyandrianarivo601@gmail.com"/>
+    <hyperlink ref="D388" r:id="rId304" display="nisokoxeno@gmail.com"/>
+    <hyperlink ref="D389" r:id="rId305" display="minorakoto32@gmail.com"/>
+    <hyperlink ref="D390" r:id="rId306" display="Gasikara42@gmail.com"/>
+    <hyperlink ref="D391" r:id="rId307" display="fanevaf47@gmail.com"/>
+    <hyperlink ref="D392" r:id="rId308" display="solofoharilalahernola@gmail.com"/>
+    <hyperlink ref="D393" r:id="rId309" display="rakotonirinamanda977@gmail.com"/>
+    <hyperlink ref="D394" r:id="rId310" display="Tinamandimbiarivo@gmail.com"/>
+    <hyperlink ref="D395" r:id="rId311" display="Stephanieraharison13@gmail.com"/>
+    <hyperlink ref="D396" r:id="rId312" display="voahariniaina117@gmail.com"/>
+    <hyperlink ref="D397" r:id="rId313" display="raisaserge1001@gmail.com"/>
+    <hyperlink ref="D398" r:id="rId314" display="ChandrineRahariniony@gmail.com"/>
+    <hyperlink ref="D399" r:id="rId315" display="rfttoussaint@gmail.com"/>
+    <hyperlink ref="D400" r:id="rId316" display="lovasoaraharimalala1@gmail.com"/>
+    <hyperlink ref="D401" r:id="rId317" display="nahfahatsiarovana@gmail.com"/>
+    <hyperlink ref="D402" r:id="rId318" display="onjacomrakoto@gmail.com"/>
+    <hyperlink ref="D403" r:id="rId319" display="ravomahefa2603@gmail.com"/>
+    <hyperlink ref="D404" r:id="rId320" display="zoly.raholinirina@gmail.com"/>
+    <hyperlink ref="D405" r:id="rId321" display="nalyravalison@gmail.com"/>
+    <hyperlink ref="D406" r:id="rId322" display="fifalianaandriamiravo@gmail.com"/>
+    <hyperlink ref="D407" r:id="rId323" display="hasinalalainarazafindrakoto@gmail.com"/>
+    <hyperlink ref="D408" r:id="rId324" display="Kiadyrandriamaharison@gmail.com"/>
+    <hyperlink ref="D409" r:id="rId325" display="alphonse.jean5236@gmail.com"/>
+    <hyperlink ref="D410" r:id="rId326" display="andonirinaraharimbalimiorantso@gmail.com"/>
+    <hyperlink ref="D411" r:id="rId327" display="dinanantenaina05@gmail.com"/>
+    <hyperlink ref="D412" r:id="rId328" display="miorarvk@gmail.com"/>
+    <hyperlink ref="D413" r:id="rId329" display="ebida912@gmail.com"/>
+    <hyperlink ref="E413" r:id="rId330" display="ebida912@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511811023622047" footer="0.25"/>

</xml_diff>